<commit_message>
Change in login button xpath
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C731942-461D-4587-B18F-62B74735878C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AB5DAE-96AD-424A-976A-BFC831D9254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="19" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="46" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="656">
   <si>
     <t>username</t>
   </si>
@@ -2064,6 +2064,15 @@
   </si>
   <si>
     <t>Patient</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>22/07/2025</t>
+  </si>
+  <si>
+    <t>22/06/2025</t>
   </si>
 </sst>
 </file>
@@ -3368,7 +3377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073326C8-FACB-4B5B-B1CF-ABFED8B93DBE}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -3591,7 +3600,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>09/07/2025</v>
+        <v>22/07/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -3670,7 +3679,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>09/07/2025</v>
+        <v>22/07/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>199</v>
@@ -3916,7 +3925,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45847</v>
+        <v>45860</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>103</v>
@@ -5572,8 +5581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1194F774-EACE-44AC-9C8A-A1CC70FE36E1}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5607,16 +5616,16 @@
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>323</v>
+        <v>653</v>
       </c>
       <c r="B2" t="s">
         <v>324</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>325</v>
+        <v>655</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>326</v>
+        <v>654</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>327</v>
@@ -5869,7 +5878,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6635,7 +6644,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>09/07/2025</v>
+        <v>22/07/2025</v>
       </c>
       <c r="C2" t="s">
         <v>415</v>
@@ -8395,6 +8404,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -8649,7 +8667,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
@@ -8660,16 +8678,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8688,7 +8705,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8697,12 +8714,4 @@
     <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Medication administration changes to correct flow.
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Riomed\Cellma4ClinicalAuto\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AB5DAE-96AD-424A-976A-BFC831D9254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE20C60-3E46-4C02-AD3D-CA754043E7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="46" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="658">
   <si>
     <t>username</t>
   </si>
@@ -2073,6 +2073,12 @@
   </si>
   <si>
     <t>22/06/2025</t>
+  </si>
+  <si>
+    <t>medadt_medication_status</t>
+  </si>
+  <si>
+    <t>given</t>
   </si>
 </sst>
 </file>
@@ -2439,13 +2445,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>374</v>
       </c>
@@ -2461,7 +2467,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>282</v>
       </c>
@@ -2486,13 +2492,13 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2500,7 +2506,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>200</v>
       </c>
@@ -2521,17 +2527,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2551,7 +2557,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>221</v>
       </c>
@@ -2585,15 +2591,15 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2610,7 +2616,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>221</v>
       </c>
@@ -2640,13 +2646,13 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2657,7 +2663,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>221</v>
       </c>
@@ -2681,17 +2687,17 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="19.54296875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2720,7 +2726,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -2762,20 +2768,20 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2804,7 +2810,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -2846,13 +2852,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -2860,7 +2866,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -2881,19 +2887,19 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="9" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1"/>
+    <col min="9" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2937,7 +2943,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2992,19 +2998,19 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3042,7 +3048,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3090,13 +3096,13 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -3104,7 +3110,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -3125,15 +3131,15 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3279,7 +3285,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>437</v>
       </c>
@@ -3381,17 +3387,17 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3411,7 +3417,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -3444,17 +3450,17 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3474,7 +3480,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -3507,14 +3513,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3525,7 +3531,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -3549,20 +3555,20 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3588,7 +3594,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -3600,7 +3606,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>22/07/2025</v>
+        <v>25/07/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -3629,19 +3635,19 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3667,7 +3673,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -3679,7 +3685,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>22/07/2025</v>
+        <v>25/07/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>199</v>
@@ -3707,14 +3713,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3725,7 +3731,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -3749,23 +3755,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="4" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="22.26953125" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" customWidth="1"/>
+    <col min="12" max="12" width="17.453125" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3809,7 +3815,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>212</v>
       </c>
@@ -3866,19 +3872,19 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3916,7 +3922,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>212</v>
       </c>
@@ -3925,7 +3931,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45860</v>
+        <v>45863</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>103</v>
@@ -3968,14 +3974,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3986,7 +3992,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>212</v>
       </c>
@@ -4010,12 +4016,12 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4056,7 +4062,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>231</v>
       </c>
@@ -4108,7 +4114,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4122,24 +4128,24 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4180,7 +4186,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>231</v>
       </c>
@@ -4234,13 +4240,13 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -4248,7 +4254,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>232</v>
       </c>
@@ -4269,22 +4275,22 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4319,7 +4325,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -4367,22 +4373,22 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4417,7 +4423,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -4465,13 +4471,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -4479,7 +4485,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>433</v>
       </c>
@@ -4500,17 +4506,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4530,7 +4536,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>259</v>
       </c>
@@ -4563,15 +4569,15 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4585,7 +4591,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>259</v>
       </c>
@@ -4612,13 +4618,13 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -4626,7 +4632,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>259</v>
       </c>
@@ -4647,15 +4653,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4669,7 +4675,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>268</v>
       </c>
@@ -4696,15 +4702,15 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4718,7 +4724,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>268</v>
       </c>
@@ -4739,45 +4745,44 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD9439C-0973-45AC-88BC-21584AF7E144}">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="4" width="17.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="8" max="9" width="13.7265625" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.453125" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="15" max="17" width="15.5703125" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="15" max="17" width="15.54296875" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" customWidth="1"/>
+    <col min="19" max="19" width="16.54296875" customWidth="1"/>
     <col min="20" max="21" width="16" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" customWidth="1"/>
+    <col min="22" max="22" width="13.1796875" customWidth="1"/>
     <col min="23" max="23" width="21" customWidth="1"/>
-    <col min="24" max="24" width="13.140625" customWidth="1"/>
-    <col min="25" max="25" width="17.7109375" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" customWidth="1"/>
-    <col min="27" max="27" width="12.28515625" customWidth="1"/>
-    <col min="28" max="28" width="15.140625" customWidth="1"/>
-    <col min="29" max="29" width="28.42578125" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" customWidth="1"/>
-    <col min="31" max="31" width="17.140625" customWidth="1"/>
-    <col min="32" max="32" width="27.140625" customWidth="1"/>
-    <col min="33" max="33" width="12.85546875" customWidth="1"/>
+    <col min="24" max="24" width="13.1796875" customWidth="1"/>
+    <col min="25" max="25" width="17.7265625" customWidth="1"/>
+    <col min="26" max="26" width="13.81640625" customWidth="1"/>
+    <col min="27" max="27" width="12.26953125" customWidth="1"/>
+    <col min="28" max="28" width="15.1796875" customWidth="1"/>
+    <col min="29" max="29" width="28.453125" customWidth="1"/>
+    <col min="30" max="30" width="14.81640625" customWidth="1"/>
+    <col min="31" max="31" width="17.1796875" customWidth="1"/>
+    <col min="32" max="32" width="27.1796875" customWidth="1"/>
+    <col min="33" max="33" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -4877,8 +4882,11 @@
       <c r="AG1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH1" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -4971,6 +4979,9 @@
       </c>
       <c r="AG2" s="8" t="s">
         <v>202</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>657</v>
       </c>
     </row>
   </sheetData>
@@ -4986,14 +4997,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5004,7 +5015,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>268</v>
       </c>
@@ -5028,15 +5039,15 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5050,7 +5061,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -5077,15 +5088,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5099,7 +5110,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -5126,14 +5137,14 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5144,7 +5155,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -5168,14 +5179,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="4" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5189,7 +5200,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>278</v>
       </c>
@@ -5216,14 +5227,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="4" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5237,7 +5248,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>278</v>
       </c>
@@ -5264,14 +5275,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5282,7 +5293,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>278</v>
       </c>
@@ -5306,18 +5317,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5370,7 +5381,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>286</v>
       </c>
@@ -5433,19 +5444,19 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5510,7 +5521,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>286</v>
       </c>
@@ -5581,20 +5592,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1194F774-EACE-44AC-9C8A-A1CC70FE36E1}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="3" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="3" width="25.54296875" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5614,7 +5625,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>653</v>
       </c>
@@ -5647,29 +5658,29 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.54296875" customWidth="1"/>
+    <col min="17" max="17" width="17.1796875" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="21" max="21" width="17.7109375" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" customWidth="1"/>
-    <col min="23" max="23" width="15.5703125" customWidth="1"/>
+    <col min="21" max="21" width="17.7265625" customWidth="1"/>
+    <col min="22" max="22" width="12.81640625" customWidth="1"/>
+    <col min="23" max="23" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5740,7 +5751,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -5819,16 +5830,16 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="3" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="3" width="25.54296875" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5848,7 +5859,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>323</v>
       </c>
@@ -5881,13 +5892,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5895,7 +5906,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>323</v>
       </c>
@@ -5916,15 +5927,15 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5938,7 +5949,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>332</v>
       </c>
@@ -5966,15 +5977,15 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -5988,7 +5999,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>332</v>
       </c>
@@ -6015,14 +6026,14 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -6033,7 +6044,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>332</v>
       </c>
@@ -6057,23 +6068,23 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>337</v>
       </c>
@@ -6120,7 +6131,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>352</v>
       </c>
@@ -6180,20 +6191,20 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>364</v>
       </c>
@@ -6228,7 +6239,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>367</v>
       </c>
@@ -6276,24 +6287,24 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="10" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20.54296875" customWidth="1"/>
+    <col min="9" max="10" width="19.7265625" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="21.140625" customWidth="1"/>
+    <col min="13" max="13" width="20.54296875" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" customWidth="1"/>
+    <col min="15" max="15" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -6340,7 +6351,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>403</v>
       </c>
@@ -6403,24 +6414,24 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="10" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20.54296875" customWidth="1"/>
+    <col min="9" max="10" width="19.7265625" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="21.140625" customWidth="1"/>
+    <col min="13" max="13" width="20.54296875" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" customWidth="1"/>
+    <col min="15" max="15" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -6467,7 +6478,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>403</v>
       </c>
@@ -6528,7 +6539,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6542,14 +6553,14 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -6560,7 +6571,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -6585,22 +6596,22 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" customWidth="1"/>
+    <col min="11" max="11" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>409</v>
       </c>
@@ -6638,13 +6649,13 @@
         <v>427</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>425</v>
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>22/07/2025</v>
+        <v>25/07/2025</v>
       </c>
       <c r="C2" t="s">
         <v>415</v>
@@ -6687,18 +6698,18 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -6751,7 +6762,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>286</v>
       </c>
@@ -6815,15 +6826,15 @@
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -6837,7 +6848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>438</v>
       </c>
@@ -6864,26 +6875,26 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>442</v>
       </c>
@@ -6930,7 +6941,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>457</v>
       </c>
@@ -6994,27 +7005,27 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>442</v>
       </c>
@@ -7064,7 +7075,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>457</v>
       </c>
@@ -7131,22 +7142,22 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="21.26953125" customWidth="1"/>
+    <col min="11" max="11" width="37.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>476</v>
       </c>
@@ -7181,7 +7192,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>487</v>
       </c>
@@ -7207,7 +7218,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>495</v>
       </c>
@@ -7224,7 +7235,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>499</v>
       </c>
@@ -7244,7 +7255,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>505</v>
       </c>
@@ -7279,10 +7290,10 @@
         <v>510</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C7" s="3"/>
     </row>
   </sheetData>
@@ -7298,23 +7309,23 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>476</v>
       </c>
@@ -7358,7 +7369,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>487</v>
       </c>
@@ -7393,7 +7404,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>495</v>
       </c>
@@ -7419,7 +7430,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>499</v>
       </c>
@@ -7448,7 +7459,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>505</v>
       </c>
@@ -7505,29 +7516,29 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="17.54296875" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.54296875" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -7592,7 +7603,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>551</v>
       </c>
@@ -7651,7 +7662,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>569</v>
       </c>
@@ -7674,7 +7685,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>575</v>
       </c>
@@ -7701,32 +7712,32 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -7800,7 +7811,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>551</v>
       </c>
@@ -7871,7 +7882,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>569</v>
       </c>
@@ -7914,7 +7925,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>575</v>
       </c>
@@ -7940,7 +7951,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
     </row>
@@ -7957,27 +7968,27 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="255.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="255.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>601</v>
       </c>
@@ -8030,7 +8041,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>618</v>
       </c>
@@ -8094,7 +8105,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
@@ -8111,28 +8122,28 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>601</v>
       </c>
@@ -8191,7 +8202,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>618</v>
       </c>
@@ -8264,19 +8275,19 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="1" max="2" width="23.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -8305,7 +8316,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>200</v>
       </c>
@@ -8347,18 +8358,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -8378,7 +8389,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>200</v>
       </c>
@@ -8404,6 +8415,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8412,7 +8434,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -8667,18 +8689,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -8686,7 +8708,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8703,15 +8725,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Physical Sign optimised code
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744665EE-E96B-4789-85AC-E158BF8CEF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F700C1A0-9B11-49E9-B02B-23FA8FACFDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="45" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="64" activeTab="70" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -83,6 +83,7 @@
     <sheet name="EditTool" sheetId="69" r:id="rId68"/>
     <sheet name="AddPatientConsent" sheetId="70" r:id="rId69"/>
     <sheet name="EditPatientConsent" sheetId="71" r:id="rId70"/>
+    <sheet name="PhysicalSign" sheetId="72" r:id="rId71"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="712">
   <si>
     <t>username</t>
   </si>
@@ -2082,6 +2083,165 @@
   </si>
   <si>
     <t>testing</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Blood Pressure (35)</t>
+  </si>
+  <si>
+    <t>Blood Pressure Diastolic (mmHg)</t>
+  </si>
+  <si>
+    <t>Blood Pressure Diastolic (mmHg) (12)</t>
+  </si>
+  <si>
+    <t>Blood Pressure Systolic (mmHg)</t>
+  </si>
+  <si>
+    <t>Blood Pressure Systolic (mmHg) (mmHg )</t>
+  </si>
+  <si>
+    <t>BMI (body mass index) centile</t>
+  </si>
+  <si>
+    <t>Capillary refill time (seconds)</t>
+  </si>
+  <si>
+    <t>Foetal heart rate</t>
+  </si>
+  <si>
+    <t>Fundal height of uterus</t>
+  </si>
+  <si>
+    <t>Halo sign</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Height (cm) (cm)</t>
+  </si>
+  <si>
+    <t>Height and weight</t>
+  </si>
+  <si>
+    <t>News Score</t>
+  </si>
+  <si>
+    <t>O2 (L/Min)</t>
+  </si>
+  <si>
+    <t>Oxygen (12)</t>
+  </si>
+  <si>
+    <t>Oxygen Saturation Scale 1 (%)</t>
+  </si>
+  <si>
+    <t>Oxygen Saturation Scale 2 (%)</t>
+  </si>
+  <si>
+    <t>PEWS score</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Pulse (Beats per minute)</t>
+  </si>
+  <si>
+    <t>Pulse-resting-rate(bpm)</t>
+  </si>
+  <si>
+    <t>Respiratory Rate (Breaths per minute)</t>
+  </si>
+  <si>
+    <t>Respiratory Rate</t>
+  </si>
+  <si>
+    <t>Serum neutralization test</t>
+  </si>
+  <si>
+    <t>SPO2</t>
+  </si>
+  <si>
+    <t>Structure of epiphyseal plate</t>
+  </si>
+  <si>
+    <t>Temperature (degree C)</t>
+  </si>
+  <si>
+    <t>Weight (kg) (kg)</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>298</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>58</t>
   </si>
 </sst>
 </file>
@@ -2135,7 +2295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2160,6 +2320,9 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3609,7 +3772,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>29/07/2025</v>
+        <v>04/08/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -3688,7 +3851,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>29/07/2025</v>
+        <v>04/08/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>199</v>
@@ -3934,7 +4097,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45867</v>
+        <v>45873</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>103</v>
@@ -5891,7 +6054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A0A6C0-CF2F-48B8-BAC5-F3E5690001A5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -6664,7 +6827,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>29/07/2025</v>
+        <v>04/08/2025</v>
       </c>
       <c r="C2" t="s">
         <v>415</v>
@@ -8276,6 +8439,265 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847F356E-F54A-4994-9714-D3DDDBAEB896}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>659</v>
+      </c>
+      <c r="B1" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>711</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82EC7FC3-A185-46F7-A2D4-55C9E247ADD9}">
   <dimension ref="A1:I2"/>
@@ -8424,6 +8846,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -8678,7 +9109,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
@@ -8689,16 +9120,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8717,7 +9147,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8726,12 +9156,4 @@
     <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
risk factor question change
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D3D7E8-C98F-4237-8AA1-32C66E7B41EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2005363-FA14-4FA8-9A55-26C1543A3312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="57" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="36" activeTab="42" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -1092,9 +1092,6 @@
     <t>Edit for Notes for Condition</t>
   </si>
   <si>
-    <t>Adult At Risk</t>
-  </si>
-  <si>
     <t>pad_notes</t>
   </si>
   <si>
@@ -2227,6 +2224,9 @@
   </si>
   <si>
     <t>Cochlear Implantation (7/31/2025, left)</t>
+  </si>
+  <si>
+    <t>At risk for injury</t>
   </si>
 </sst>
 </file>
@@ -2621,18 +2621,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2640,7 +2640,7 @@
         <v>280</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -3135,16 +3135,16 @@
         <v>159</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>157</v>
       </c>
       <c r="L2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M2" t="s">
         <v>188</v>
@@ -3456,22 +3456,22 @@
     </row>
     <row r="2" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>51</v>
@@ -3591,7 +3591,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C2" t="s">
         <v>131</v>
@@ -3654,7 +3654,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C2" t="s">
         <v>116</v>
@@ -3705,7 +3705,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -3989,13 +3989,13 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>102</v>
@@ -4096,7 +4096,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
@@ -4166,7 +4166,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -4499,7 +4499,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4511,7 +4511,7 @@
         <v>247</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="G2" t="s">
         <v>248</v>
@@ -4597,7 +4597,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4656,7 +4656,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B2" t="s">
         <v>255</v>
@@ -4964,7 +4964,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -5054,7 +5054,7 @@
         <v>200</v>
       </c>
       <c r="AH1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -5062,13 +5062,13 @@
         <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E2" t="s">
         <v>71</v>
@@ -5086,10 +5086,10 @@
         <v>102</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>645</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>646</v>
       </c>
       <c r="L2" t="s">
         <v>176</v>
@@ -5122,7 +5122,7 @@
         <v>82</v>
       </c>
       <c r="X2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="Y2" t="s">
         <v>104</v>
@@ -5152,7 +5152,7 @@
         <v>201</v>
       </c>
       <c r="AH2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -5207,7 +5207,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5237,7 +5237,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>328</v>
+        <v>706</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>269</v>
@@ -5286,7 +5286,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>328</v>
+        <v>706</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>272</v>
@@ -5304,8 +5304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3F2689-A05C-47BB-9880-495021A0BDBF}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5331,7 +5331,7 @@
         <v>267</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>328</v>
+        <v>706</v>
       </c>
       <c r="C2" t="s">
         <v>273</v>
@@ -5376,7 +5376,7 @@
         <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>278</v>
@@ -5424,7 +5424,7 @@
         <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>277</v>
@@ -5469,7 +5469,7 @@
         <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C2" t="s">
         <v>279</v>
@@ -5798,16 +5798,16 @@
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B2" t="s">
         <v>322</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>325</v>
@@ -5862,7 +5862,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -5934,7 +5934,7 @@
         <v>112</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E2" t="s">
         <v>86</v>
@@ -6088,7 +6088,7 @@
         <v>322</v>
       </c>
       <c r="C2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -6123,21 +6123,21 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>331</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>332</v>
-      </c>
-      <c r="D2" t="s">
-        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -6173,21 +6173,21 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>331</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>332</v>
-      </c>
-      <c r="D2" t="s">
-        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -6223,13 +6223,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>331</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -6263,96 +6263,96 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" t="s">
         <v>335</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>336</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>337</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>338</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>339</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>340</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>341</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>342</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>343</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>344</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>345</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>346</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>347</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>348</v>
-      </c>
-      <c r="O1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" t="s">
         <v>354</v>
       </c>
-      <c r="F2" t="s">
-        <v>355</v>
-      </c>
       <c r="G2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H2" t="s">
         <v>98</v>
       </c>
       <c r="I2" t="s">
+        <v>355</v>
+      </c>
+      <c r="J2" t="s">
         <v>356</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>357</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>358</v>
-      </c>
-      <c r="L2" t="s">
-        <v>359</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>318</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="O2" t="s">
         <v>360</v>
-      </c>
-      <c r="O2" t="s">
-        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -6383,72 +6383,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" t="s">
         <v>362</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G1" t="s">
         <v>363</v>
-      </c>
-      <c r="C1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D1" t="s">
-        <v>341</v>
-      </c>
-      <c r="E1" t="s">
-        <v>342</v>
-      </c>
-      <c r="F1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G1" t="s">
-        <v>364</v>
       </c>
       <c r="H1" t="s">
         <v>300</v>
       </c>
       <c r="I1" t="s">
+        <v>346</v>
+      </c>
+      <c r="J1" t="s">
         <v>347</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>348</v>
-      </c>
-      <c r="K1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>366</v>
-      </c>
       <c r="C2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E2" t="s">
         <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>318</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="K2" t="s">
         <v>360</v>
-      </c>
-      <c r="K2" t="s">
-        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -6489,93 +6489,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" t="s">
         <v>376</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>377</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>378</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>379</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>380</v>
       </c>
-      <c r="H1" t="s">
-        <v>381</v>
-      </c>
       <c r="I1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N1" t="s">
+        <v>397</v>
+      </c>
+      <c r="O1" t="s">
         <v>398</v>
-      </c>
-      <c r="O1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C2" t="s">
+        <v>381</v>
+      </c>
+      <c r="D2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F2" t="s">
+        <v>384</v>
+      </c>
+      <c r="G2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H2" t="s">
+        <v>386</v>
+      </c>
+      <c r="I2" t="s">
+        <v>388</v>
+      </c>
+      <c r="J2" t="s">
+        <v>390</v>
+      </c>
+      <c r="K2" t="s">
+        <v>392</v>
+      </c>
+      <c r="L2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M2" t="s">
+        <v>396</v>
+      </c>
+      <c r="N2" t="s">
         <v>401</v>
       </c>
-      <c r="B2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C2" t="s">
-        <v>382</v>
-      </c>
-      <c r="D2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E2" t="s">
-        <v>384</v>
-      </c>
-      <c r="F2" t="s">
-        <v>385</v>
-      </c>
-      <c r="G2" t="s">
-        <v>386</v>
-      </c>
-      <c r="H2" t="s">
-        <v>387</v>
-      </c>
-      <c r="I2" t="s">
-        <v>389</v>
-      </c>
-      <c r="J2" t="s">
-        <v>391</v>
-      </c>
-      <c r="K2" t="s">
-        <v>393</v>
-      </c>
-      <c r="L2" t="s">
-        <v>395</v>
-      </c>
-      <c r="M2" t="s">
-        <v>397</v>
-      </c>
-      <c r="N2" t="s">
-        <v>402</v>
-      </c>
       <c r="O2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -6616,93 +6616,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" t="s">
         <v>376</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>377</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>378</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>379</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>380</v>
       </c>
-      <c r="H1" t="s">
-        <v>381</v>
-      </c>
       <c r="I1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N1" t="s">
+        <v>397</v>
+      </c>
+      <c r="O1" t="s">
         <v>398</v>
-      </c>
-      <c r="O1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C2" t="s">
+        <v>381</v>
+      </c>
+      <c r="D2" t="s">
         <v>382</v>
       </c>
-      <c r="D2" t="s">
-        <v>383</v>
-      </c>
       <c r="E2" t="s">
+        <v>402</v>
+      </c>
+      <c r="F2" t="s">
+        <v>384</v>
+      </c>
+      <c r="G2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H2" t="s">
         <v>403</v>
       </c>
-      <c r="F2" t="s">
-        <v>385</v>
-      </c>
-      <c r="G2" t="s">
-        <v>386</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>388</v>
+      </c>
+      <c r="J2" t="s">
+        <v>390</v>
+      </c>
+      <c r="K2" t="s">
         <v>404</v>
       </c>
-      <c r="I2" t="s">
-        <v>389</v>
-      </c>
-      <c r="J2" t="s">
-        <v>391</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M2" t="s">
+        <v>396</v>
+      </c>
+      <c r="N2" t="s">
         <v>405</v>
       </c>
-      <c r="L2" t="s">
-        <v>395</v>
-      </c>
-      <c r="M2" t="s">
-        <v>397</v>
-      </c>
-      <c r="N2" t="s">
-        <v>406</v>
-      </c>
       <c r="O2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -6790,55 +6790,55 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B1" t="s">
         <v>407</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>408</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>409</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>410</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>411</v>
       </c>
-      <c r="F1" t="s">
-        <v>412</v>
-      </c>
       <c r="G1" t="s">
+        <v>414</v>
+      </c>
+      <c r="H1" t="s">
         <v>415</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>416</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>417</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>418</v>
       </c>
-      <c r="K1" t="s">
-        <v>419</v>
-      </c>
       <c r="L1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
         <v>13/10/2025</v>
       </c>
       <c r="C2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D2" t="s">
         <v>413</v>
-      </c>
-      <c r="D2" t="s">
-        <v>414</v>
       </c>
       <c r="E2" t="s">
         <v>304</v>
@@ -6847,19 +6847,19 @@
         <v>116</v>
       </c>
       <c r="H2" t="s">
+        <v>419</v>
+      </c>
+      <c r="I2" t="s">
         <v>420</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>421</v>
       </c>
-      <c r="J2" t="s">
-        <v>422</v>
-      </c>
       <c r="K2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -7027,16 +7027,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>437</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -7048,7 +7048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251B21E0-6337-4D24-89BA-CCC72B4CE178}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -7073,66 +7073,66 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B1" t="s">
         <v>439</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>440</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>441</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>442</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>443</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>444</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>445</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>446</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>447</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>448</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>449</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>450</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>451</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>452</v>
-      </c>
-      <c r="O1" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B2" t="s">
         <v>454</v>
       </c>
-      <c r="B2" t="s">
-        <v>455</v>
-      </c>
       <c r="C2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>457</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>458</v>
       </c>
       <c r="F2" t="str">
         <f>LOWER(G2)</f>
@@ -7146,7 +7146,7 @@
         <v>internal</v>
       </c>
       <c r="I2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J2" t="str">
         <f>LOWER(K2)</f>
@@ -7156,17 +7156,17 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="M2" t="str">
         <f>LOWER(N2)</f>
         <v>implanted</v>
       </c>
       <c r="N2" t="s">
+        <v>460</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>461</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -7204,86 +7204,86 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B1" t="s">
         <v>439</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>440</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>441</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F1" t="s">
         <v>442</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H1" t="s">
+        <v>444</v>
+      </c>
+      <c r="I1" t="s">
+        <v>445</v>
+      </c>
+      <c r="J1" t="s">
+        <v>446</v>
+      </c>
+      <c r="K1" t="s">
+        <v>447</v>
+      </c>
+      <c r="L1" t="s">
+        <v>448</v>
+      </c>
+      <c r="M1" t="s">
+        <v>449</v>
+      </c>
+      <c r="N1" t="s">
+        <v>450</v>
+      </c>
+      <c r="O1" t="s">
+        <v>451</v>
+      </c>
+      <c r="P1" t="s">
         <v>463</v>
-      </c>
-      <c r="F1" t="s">
-        <v>443</v>
-      </c>
-      <c r="G1" t="s">
-        <v>444</v>
-      </c>
-      <c r="H1" t="s">
-        <v>445</v>
-      </c>
-      <c r="I1" t="s">
-        <v>446</v>
-      </c>
-      <c r="J1" t="s">
-        <v>447</v>
-      </c>
-      <c r="K1" t="s">
-        <v>448</v>
-      </c>
-      <c r="L1" t="s">
-        <v>449</v>
-      </c>
-      <c r="M1" t="s">
-        <v>450</v>
-      </c>
-      <c r="N1" t="s">
-        <v>451</v>
-      </c>
-      <c r="O1" t="s">
-        <v>452</v>
-      </c>
-      <c r="P1" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B2" t="s">
+        <v>464</v>
+      </c>
+      <c r="C2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D2" t="s">
         <v>465</v>
       </c>
-      <c r="C2" t="s">
-        <v>456</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>466</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="6" t="s">
         <v>467</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>468</v>
       </c>
       <c r="G2" t="str">
         <f>SUBSTITUTE(LOWER(H2)," ","")</f>
         <v>firststage</v>
       </c>
       <c r="H2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I2" t="str">
         <f>LOWER(J2)</f>
         <v>external</v>
       </c>
       <c r="J2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K2" t="str">
         <f>LOWER(L2)</f>
@@ -7293,7 +7293,7 @@
         <v>184</v>
       </c>
       <c r="M2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="N2" t="str">
         <f>LOWER(O2)</f>
@@ -7303,7 +7303,7 @@
         <v>205</v>
       </c>
       <c r="P2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -7336,126 +7336,126 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B1" t="s">
         <v>473</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>474</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>475</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>476</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>477</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>478</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>479</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>480</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>481</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>482</v>
-      </c>
-      <c r="K1" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B2" t="s">
         <v>484</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>485</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>486</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>487</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>488</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>489</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>490</v>
-      </c>
-      <c r="K2" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B3" t="s">
         <v>492</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>493</v>
-      </c>
-      <c r="C3" t="s">
-        <v>494</v>
       </c>
       <c r="D3" t="s">
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>495</v>
+      </c>
+      <c r="B4" t="s">
         <v>496</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>497</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>498</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>499</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>500</v>
-      </c>
-      <c r="K4" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B5" t="s">
         <v>502</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" t="s">
         <v>504</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>505</v>
       </c>
-      <c r="E5" t="s">
-        <v>506</v>
-      </c>
       <c r="F5" t="s">
+        <v>502</v>
+      </c>
+      <c r="G5" t="s">
         <v>503</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>504</v>
-      </c>
-      <c r="H5" t="s">
-        <v>505</v>
       </c>
       <c r="I5" t="s">
         <v>100</v>
@@ -7464,7 +7464,7 @@
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7504,43 +7504,43 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B1" t="s">
         <v>473</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>474</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>475</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>476</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>477</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>478</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>479</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>480</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>481</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>482</v>
       </c>
-      <c r="K1" t="s">
-        <v>483</v>
-      </c>
       <c r="L1" t="s">
+        <v>507</v>
+      </c>
+      <c r="M1" t="s">
         <v>508</v>
-      </c>
-      <c r="M1" t="s">
-        <v>509</v>
       </c>
       <c r="N1" t="s">
         <v>122</v>
@@ -7548,118 +7548,118 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C2" t="s">
         <v>510</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>511</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>512</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>513</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>514</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>515</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="N2" t="s">
         <v>517</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="N2" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B3" t="s">
+        <v>518</v>
+      </c>
+      <c r="C3" t="s">
         <v>519</v>
-      </c>
-      <c r="C3" t="s">
-        <v>520</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L3" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="N3" t="s">
         <v>517</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="N3" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B4" t="s">
+        <v>521</v>
+      </c>
+      <c r="C4" t="s">
         <v>522</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>523</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>524</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>525</v>
       </c>
-      <c r="K4" t="s">
-        <v>526</v>
-      </c>
       <c r="L4" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="N4" t="s">
         <v>517</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="N4" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="C5" t="s">
+        <v>504</v>
+      </c>
+      <c r="D5" t="s">
+        <v>505</v>
+      </c>
+      <c r="E5" t="s">
         <v>502</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="F5" t="s">
+        <v>503</v>
+      </c>
+      <c r="G5" t="s">
         <v>504</v>
       </c>
-      <c r="C5" t="s">
-        <v>505</v>
-      </c>
-      <c r="D5" t="s">
-        <v>506</v>
-      </c>
-      <c r="E5" t="s">
-        <v>503</v>
-      </c>
-      <c r="F5" t="s">
-        <v>504</v>
-      </c>
-      <c r="G5" t="s">
-        <v>505</v>
-      </c>
       <c r="H5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I5" t="s">
         <v>60</v>
@@ -7668,16 +7668,16 @@
         <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L5" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="N5" t="s">
         <v>517</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="N5" t="s">
-        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -7720,160 +7720,160 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1" t="s">
         <v>528</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>529</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>530</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>531</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>532</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>533</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>534</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>535</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>536</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>537</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>538</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>539</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>540</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>541</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>542</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>543</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>544</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>545</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>546</v>
-      </c>
-      <c r="U1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B2" t="s">
         <v>548</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>549</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>550</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>551</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>552</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>553</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>554</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>555</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>556</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>557</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>558</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>559</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>560</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>561</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>562</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>563</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>564</v>
       </c>
-      <c r="S2" t="s">
-        <v>565</v>
-      </c>
       <c r="U2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>565</v>
+      </c>
+      <c r="B3" t="s">
         <v>566</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>567</v>
-      </c>
-      <c r="C3" t="s">
-        <v>568</v>
       </c>
       <c r="D3" t="s">
         <v>316</v>
       </c>
       <c r="O3" t="s">
+        <v>568</v>
+      </c>
+      <c r="T3" t="s">
         <v>569</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>570</v>
-      </c>
-      <c r="U3" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>571</v>
+      </c>
+      <c r="O4" t="s">
         <v>572</v>
       </c>
-      <c r="O4" t="s">
+      <c r="T4" t="s">
         <v>573</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>574</v>
-      </c>
-      <c r="U4" t="s">
-        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -7919,70 +7919,70 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1" t="s">
         <v>528</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>529</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>530</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>531</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>532</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>533</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>534</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>535</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>536</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>537</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>538</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>539</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>540</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>541</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>542</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>543</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>544</v>
       </c>
-      <c r="S1" t="s">
-        <v>545</v>
-      </c>
       <c r="T1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="U1" t="s">
         <v>132</v>
       </c>
       <c r="V1" t="s">
+        <v>575</v>
+      </c>
+      <c r="W1" t="s">
         <v>576</v>
-      </c>
-      <c r="W1" t="s">
-        <v>577</v>
       </c>
       <c r="X1" t="s">
         <v>122</v>
@@ -7990,93 +7990,93 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B2" t="s">
+        <v>552</v>
+      </c>
+      <c r="C2" t="s">
+        <v>553</v>
+      </c>
+      <c r="D2" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2" t="s">
+        <v>578</v>
+      </c>
+      <c r="F2" t="s">
         <v>548</v>
       </c>
-      <c r="B2" t="s">
-        <v>553</v>
-      </c>
-      <c r="C2" t="s">
-        <v>554</v>
-      </c>
-      <c r="D2" t="s">
-        <v>578</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H2" t="s">
         <v>579</v>
       </c>
-      <c r="F2" t="s">
-        <v>549</v>
-      </c>
-      <c r="G2" t="s">
-        <v>550</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>558</v>
+      </c>
+      <c r="J2" t="s">
+        <v>559</v>
+      </c>
+      <c r="K2" t="s">
         <v>580</v>
       </c>
-      <c r="I2" t="s">
-        <v>559</v>
-      </c>
-      <c r="J2" t="s">
-        <v>560</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>555</v>
+      </c>
+      <c r="M2" t="s">
+        <v>556</v>
+      </c>
+      <c r="N2" t="s">
         <v>581</v>
       </c>
-      <c r="L2" t="s">
-        <v>556</v>
-      </c>
-      <c r="M2" t="s">
-        <v>557</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>582</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>583</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>584</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>585</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>547</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>586</v>
       </c>
-      <c r="T2" t="s">
-        <v>548</v>
-      </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="X2" t="s">
         <v>587</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="X2" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>589</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>590</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>591</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>186</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -8087,45 +8087,45 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="T3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="V3" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="X3" t="s">
         <v>587</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="X3" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>594</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="O4" t="s">
         <v>595</v>
       </c>
-      <c r="O4" t="s">
+      <c r="T4" t="s">
+        <v>574</v>
+      </c>
+      <c r="V4" s="5" t="s">
         <v>596</v>
       </c>
-      <c r="T4" t="s">
-        <v>575</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>597</v>
-      </c>
       <c r="W4" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="X4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -8167,108 +8167,108 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B1" t="s">
         <v>598</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>599</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>600</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>601</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>602</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>603</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>604</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>605</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>606</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>607</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>608</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>609</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>610</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>611</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>612</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>613</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2" t="s">
         <v>615</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>616</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="6" t="s">
         <v>617</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>618</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" t="s">
         <v>619</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>620</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>621</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>622</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>623</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>624</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>625</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>626</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>627</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>628</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>629</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="10" t="s">
         <v>630</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -8322,121 +8322,121 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B1" t="s">
         <v>598</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>631</v>
+      </c>
+      <c r="D1" t="s">
         <v>599</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>600</v>
+      </c>
+      <c r="F1" t="s">
+        <v>601</v>
+      </c>
+      <c r="G1" t="s">
         <v>632</v>
       </c>
-      <c r="D1" t="s">
-        <v>600</v>
-      </c>
-      <c r="E1" t="s">
-        <v>601</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>602</v>
       </c>
-      <c r="G1" t="s">
-        <v>633</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>603</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>604</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>605</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>606</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>607</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>608</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>609</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>610</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>611</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>612</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>613</v>
-      </c>
-      <c r="S1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2" t="s">
         <v>615</v>
       </c>
-      <c r="B2" t="s">
-        <v>616</v>
-      </c>
       <c r="C2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D2" t="str">
         <f>LOWER(C2)</f>
         <v>withdrawn</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H2" t="s">
+        <v>619</v>
+      </c>
+      <c r="I2" t="s">
         <v>620</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>621</v>
       </c>
-      <c r="J2" t="s">
-        <v>622</v>
-      </c>
       <c r="K2" t="s">
+        <v>634</v>
+      </c>
+      <c r="L2" t="s">
         <v>635</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>636</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>637</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>638</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>639</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>640</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>641</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" s="10" t="s">
         <v>642</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -8460,47 +8460,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B1" t="s">
         <v>653</v>
-      </c>
-      <c r="B1" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>82</v>
@@ -8508,143 +8508,143 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>316</v>
@@ -8652,26 +8652,26 @@
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change risk factor question
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2005363-FA14-4FA8-9A55-26C1543A3312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785A3BB9-4DA6-439E-9EE0-347E1D04D1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="36" activeTab="42" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2226,7 +2226,7 @@
     <t>Cochlear Implantation (7/31/2025, left)</t>
   </si>
   <si>
-    <t>At risk for injury</t>
+    <t>Child at risk</t>
   </si>
 </sst>
 </file>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>13/10/2025</v>
+        <v>14/10/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -3854,7 +3854,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>13/10/2025</v>
+        <v>14/10/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -4100,7 +4100,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45943</v>
+        <v>45944</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>102</v>
@@ -5256,7 +5256,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5305,7 +5305,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6832,7 +6832,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>13/10/2025</v>
+        <v>14/10/2025</v>
       </c>
       <c r="C2" t="s">
         <v>412</v>
@@ -8828,6 +8828,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9082,27 +9102,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9119,23 +9138,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Push Alert code and User changes
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BE4B4F-1CEE-4059-A419-C22785D31D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF546072-FD5E-4B02-A1C9-F7CD76061E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="57" activeTab="62" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="707">
   <si>
     <t>username</t>
   </si>
@@ -2220,10 +2220,13 @@
     <t>01/07/2025</t>
   </si>
   <si>
-    <t>s.d</t>
-  </si>
-  <si>
     <t>Child at risk</t>
+  </si>
+  <si>
+    <t>manoj.automation</t>
+  </si>
+  <si>
+    <t>Manoj@2025</t>
   </si>
 </sst>
 </file>
@@ -2598,8 +2601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE4FC9F-2982-4FD6-8BD6-4330FF8DA2DE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,18 +2621,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>371</v>
+        <v>705</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>372</v>
+        <v>706</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>704</v>
+        <v>371</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>428</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2643,8 +2646,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{0C05B6B9-5554-4DE8-9F6A-6002C7FF4022}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{D4AE188D-9B09-40C0-AC46-716391123A5D}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{511CBB1F-6895-4824-9854-87E0171EA2FB}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{D4AE188D-9B09-40C0-AC46-716391123A5D}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{511CBB1F-6895-4824-9854-87E0171EA2FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3772,7 +3775,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>14/10/2025</v>
+        <v>16/10/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -3851,7 +3854,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>14/10/2025</v>
+        <v>16/10/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -4097,7 +4100,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45944</v>
+        <v>45946</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>102</v>
@@ -5234,7 +5237,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>269</v>
@@ -5283,7 +5286,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>272</v>
@@ -5328,7 +5331,7 @@
         <v>267</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C2" t="s">
         <v>273</v>
@@ -6829,7 +6832,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>14/10/2025</v>
+        <v>16/10/2025</v>
       </c>
       <c r="C2" t="s">
         <v>412</v>
@@ -7045,7 +7048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251B21E0-6337-4D24-89BA-CCC72B4CE178}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -8825,17 +8828,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8844,7 +8836,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9099,18 +9091,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -9118,7 +9110,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9135,4 +9127,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Patient summary for linux
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78412845-67C7-478F-9674-69CF4AC676B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FECE0F2-889F-44D3-A3AD-06D63749AFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="722">
   <si>
     <t>username</t>
   </si>
@@ -1158,9 +1158,6 @@
     <t>Regular Checkup</t>
   </si>
   <si>
-    <t>20/08/2024</t>
-  </si>
-  <si>
     <t>09:00</t>
   </si>
   <si>
@@ -1200,12 +1197,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>22/08/2024</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
     <t>Task Updated</t>
   </si>
   <si>
@@ -2227,6 +2218,60 @@
   </si>
   <si>
     <t>Manoj@2025</t>
+  </si>
+  <si>
+    <t>task_category</t>
+  </si>
+  <si>
+    <t>existing_task_search</t>
+  </si>
+  <si>
+    <t>Abacavir 600mg / Lamivudine 300mg tablets</t>
+  </si>
+  <si>
+    <t>task_type</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>task_description</t>
+  </si>
+  <si>
+    <t>Added for testing</t>
+  </si>
+  <si>
+    <t>task_action_perform</t>
+  </si>
+  <si>
+    <t>local_code</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Add Record</t>
+  </si>
+  <si>
+    <t>Updates for testing</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Prerelease</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>hosp2560</t>
   </si>
 </sst>
 </file>
@@ -2286,7 +2331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2316,6 +2361,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2601,7 +2649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE4FC9F-2982-4FD6-8BD6-4330FF8DA2DE}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -2621,26 +2669,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2648,7 +2696,7 @@
         <v>280</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -3144,16 +3192,16 @@
         <v>159</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>157</v>
       </c>
       <c r="L2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="M2" t="s">
         <v>188</v>
@@ -3303,10 +3351,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF0DF87-67F2-4E87-A7EE-C4365800D834}">
-  <dimension ref="A1:AV2"/>
+  <dimension ref="A1:AV8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,22 +3513,22 @@
     </row>
     <row r="2" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>702</v>
+        <v>721</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>433</v>
+        <v>720</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>701</v>
+        <v>719</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>700</v>
+        <v>433</v>
+      </c>
+      <c r="I2" s="17">
+        <v>36161</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>51</v>
@@ -3549,6 +3597,95 @@
         <v>65</v>
       </c>
       <c r="AV2" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>699</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>698</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>697</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W8" s="2">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV8" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3600,7 +3737,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C2" t="s">
         <v>131</v>
@@ -3663,7 +3800,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C2" t="s">
         <v>116</v>
@@ -3714,7 +3851,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -3784,7 +3921,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>22/10/2025</v>
+        <v>28/10/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -3863,7 +4000,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>22/10/2025</v>
+        <v>28/10/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -3998,13 +4135,13 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>102</v>
@@ -4105,11 +4242,11 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45952</v>
+        <v>45958</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>102</v>
@@ -4175,7 +4312,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -4508,7 +4645,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4520,7 +4657,7 @@
         <v>247</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="G2" t="s">
         <v>248</v>
@@ -4606,7 +4743,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4665,7 +4802,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B2" t="s">
         <v>255</v>
@@ -4973,7 +5110,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -5063,7 +5200,7 @@
         <v>200</v>
       </c>
       <c r="AH1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -5071,13 +5208,13 @@
         <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E2" t="s">
         <v>71</v>
@@ -5095,10 +5232,10 @@
         <v>102</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="L2" t="s">
         <v>176</v>
@@ -5131,7 +5268,7 @@
         <v>82</v>
       </c>
       <c r="X2" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="Y2" t="s">
         <v>104</v>
@@ -5161,7 +5298,7 @@
         <v>201</v>
       </c>
       <c r="AH2" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
   </sheetData>
@@ -5246,7 +5383,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>269</v>
@@ -5295,7 +5432,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>272</v>
@@ -5340,7 +5477,7 @@
         <v>267</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="C2" t="s">
         <v>273</v>
@@ -5385,7 +5522,7 @@
         <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>278</v>
@@ -5433,7 +5570,7 @@
         <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>277</v>
@@ -5478,7 +5615,7 @@
         <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
         <v>279</v>
@@ -5807,16 +5944,16 @@
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="B2" t="s">
         <v>322</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>325</v>
@@ -5871,7 +6008,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -5943,7 +6080,7 @@
         <v>112</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E2" t="s">
         <v>86</v>
@@ -6097,7 +6234,7 @@
         <v>322</v>
       </c>
       <c r="C2" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
   </sheetData>
@@ -6248,120 +6385,157 @@
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6C2239-2180-4B9C-B8A1-E16F3FCE77A5}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B1" t="s">
+        <v>705</v>
+      </c>
+      <c r="C1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D1" t="s">
+        <v>709</v>
+      </c>
+      <c r="E1" t="s">
+        <v>711</v>
+      </c>
+      <c r="F1" t="s">
+        <v>712</v>
+      </c>
+      <c r="G1" t="s">
         <v>334</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>335</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>336</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>337</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>338</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>339</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>340</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>341</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>342</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>343</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>344</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>345</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>346</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>347</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2" t="s">
+        <v>708</v>
+      </c>
+      <c r="D2" t="s">
+        <v>710</v>
+      </c>
+      <c r="E2" t="s">
+        <v>718</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="G2" t="s">
         <v>349</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="H2" s="9" t="str">
+        <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
+        <v>28/10/2025</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="L2" t="s">
         <v>353</v>
       </c>
-      <c r="F2" t="s">
+      <c r="M2" t="s">
+        <v>364</v>
+      </c>
+      <c r="N2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" t="s">
         <v>354</v>
       </c>
-      <c r="G2" t="s">
-        <v>367</v>
-      </c>
-      <c r="H2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="P2" t="s">
         <v>355</v>
       </c>
-      <c r="J2" t="s">
+      <c r="Q2" t="s">
         <v>356</v>
       </c>
-      <c r="K2" t="s">
+      <c r="R2" t="s">
         <v>357</v>
       </c>
-      <c r="L2" t="s">
+      <c r="S2" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="U2" t="s">
         <v>359</v>
-      </c>
-      <c r="O2" t="s">
-        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -6371,93 +6545,138 @@
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B730A7AF-1268-4970-A808-63C4CFDE9D42}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B1" t="s">
+        <v>705</v>
+      </c>
+      <c r="C1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D1" t="s">
+        <v>709</v>
+      </c>
+      <c r="E1" t="s">
+        <v>711</v>
+      </c>
+      <c r="F1" t="s">
+        <v>712</v>
+      </c>
+      <c r="G1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H1" t="s">
+        <v>360</v>
+      </c>
+      <c r="I1" t="s">
         <v>361</v>
       </c>
-      <c r="B1" t="s">
+      <c r="J1" t="s">
+        <v>339</v>
+      </c>
+      <c r="K1" t="s">
+        <v>340</v>
+      </c>
+      <c r="L1" t="s">
+        <v>341</v>
+      </c>
+      <c r="M1" t="s">
+        <v>342</v>
+      </c>
+      <c r="N1" t="s">
         <v>362</v>
       </c>
-      <c r="C1" t="s">
-        <v>339</v>
-      </c>
-      <c r="D1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F1" t="s">
-        <v>342</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
+        <v>300</v>
+      </c>
+      <c r="P1" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>347</v>
+      </c>
+      <c r="R1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2" t="s">
+        <v>708</v>
+      </c>
+      <c r="D2" t="s">
+        <v>715</v>
+      </c>
+      <c r="E2" t="s">
+        <v>714</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="G2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H2" s="9" t="str">
+        <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
+        <v>28/10/2025</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="J2" t="s">
+        <v>353</v>
+      </c>
+      <c r="K2" t="s">
+        <v>364</v>
+      </c>
+      <c r="L2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" t="s">
+        <v>354</v>
+      </c>
+      <c r="N2" t="s">
+        <v>356</v>
+      </c>
+      <c r="O2" t="s">
         <v>363</v>
       </c>
-      <c r="H1" t="s">
-        <v>300</v>
-      </c>
-      <c r="I1" t="s">
-        <v>346</v>
-      </c>
-      <c r="J1" t="s">
-        <v>347</v>
-      </c>
-      <c r="K1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="C2" t="s">
-        <v>354</v>
-      </c>
-      <c r="D2" t="s">
-        <v>367</v>
-      </c>
-      <c r="E2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" t="s">
-        <v>355</v>
-      </c>
-      <c r="G2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H2" t="s">
-        <v>366</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="R2" t="s">
         <v>359</v>
-      </c>
-      <c r="K2" t="s">
-        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -6498,93 +6717,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F1" t="s">
         <v>375</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>376</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>377</v>
       </c>
-      <c r="F1" t="s">
-        <v>378</v>
-      </c>
-      <c r="G1" t="s">
-        <v>379</v>
-      </c>
-      <c r="H1" t="s">
-        <v>380</v>
-      </c>
       <c r="I1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="J1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="L1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="M1" t="s">
+        <v>392</v>
+      </c>
+      <c r="N1" t="s">
+        <v>394</v>
+      </c>
+      <c r="O1" t="s">
         <v>395</v>
-      </c>
-      <c r="N1" t="s">
-        <v>397</v>
-      </c>
-      <c r="O1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E2" t="s">
+        <v>380</v>
+      </c>
+      <c r="F2" t="s">
         <v>381</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>382</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>383</v>
       </c>
-      <c r="F2" t="s">
-        <v>384</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>385</v>
       </c>
-      <c r="H2" t="s">
-        <v>386</v>
-      </c>
-      <c r="I2" t="s">
-        <v>388</v>
-      </c>
       <c r="J2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="K2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="L2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="M2" t="s">
+        <v>393</v>
+      </c>
+      <c r="N2" t="s">
+        <v>398</v>
+      </c>
+      <c r="O2" t="s">
         <v>396</v>
       </c>
-      <c r="N2" t="s">
-        <v>401</v>
-      </c>
-      <c r="O2" t="s">
-        <v>399</v>
-      </c>
       <c r="P2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -6625,93 +6844,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F1" t="s">
         <v>375</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>376</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>377</v>
       </c>
-      <c r="F1" t="s">
-        <v>378</v>
-      </c>
-      <c r="G1" t="s">
-        <v>379</v>
-      </c>
-      <c r="H1" t="s">
-        <v>380</v>
-      </c>
       <c r="I1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="J1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="L1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="M1" t="s">
+        <v>392</v>
+      </c>
+      <c r="N1" t="s">
+        <v>394</v>
+      </c>
+      <c r="O1" t="s">
         <v>395</v>
-      </c>
-      <c r="N1" t="s">
-        <v>397</v>
-      </c>
-      <c r="O1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F2" t="s">
+        <v>381</v>
+      </c>
+      <c r="G2" t="s">
+        <v>382</v>
+      </c>
+      <c r="H2" t="s">
         <v>400</v>
       </c>
-      <c r="B2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C2" t="s">
-        <v>381</v>
-      </c>
-      <c r="D2" t="s">
-        <v>382</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
+        <v>385</v>
+      </c>
+      <c r="J2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K2" t="s">
+        <v>401</v>
+      </c>
+      <c r="L2" t="s">
+        <v>391</v>
+      </c>
+      <c r="M2" t="s">
+        <v>393</v>
+      </c>
+      <c r="N2" t="s">
         <v>402</v>
       </c>
-      <c r="F2" t="s">
-        <v>384</v>
-      </c>
-      <c r="G2" t="s">
-        <v>385</v>
-      </c>
-      <c r="H2" t="s">
-        <v>403</v>
-      </c>
-      <c r="I2" t="s">
-        <v>388</v>
-      </c>
-      <c r="J2" t="s">
-        <v>390</v>
-      </c>
-      <c r="K2" t="s">
-        <v>404</v>
-      </c>
-      <c r="L2" t="s">
-        <v>394</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>396</v>
       </c>
-      <c r="N2" t="s">
-        <v>405</v>
-      </c>
-      <c r="O2" t="s">
-        <v>399</v>
-      </c>
       <c r="P2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -6799,55 +7018,55 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D1" t="s">
         <v>406</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>407</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>408</v>
       </c>
-      <c r="D1" t="s">
-        <v>409</v>
-      </c>
-      <c r="E1" t="s">
-        <v>410</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>411</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>412</v>
+      </c>
+      <c r="I1" t="s">
+        <v>413</v>
+      </c>
+      <c r="J1" t="s">
         <v>414</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>415</v>
       </c>
-      <c r="I1" t="s">
-        <v>416</v>
-      </c>
-      <c r="J1" t="s">
-        <v>417</v>
-      </c>
-      <c r="K1" t="s">
-        <v>418</v>
-      </c>
       <c r="L1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>22/10/2025</v>
+        <v>28/10/2025</v>
       </c>
       <c r="C2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D2" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E2" t="s">
         <v>304</v>
@@ -6856,19 +7075,19 @@
         <v>116</v>
       </c>
       <c r="H2" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I2" t="s">
+        <v>417</v>
+      </c>
+      <c r="J2" t="s">
+        <v>418</v>
+      </c>
+      <c r="K2" t="s">
         <v>420</v>
       </c>
-      <c r="J2" t="s">
-        <v>421</v>
-      </c>
-      <c r="K2" t="s">
-        <v>423</v>
-      </c>
       <c r="L2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -7036,16 +7255,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>434</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -7082,66 +7301,66 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1" t="s">
         <v>438</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>439</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>440</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>441</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>442</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>443</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>444</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>445</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>446</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>447</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>448</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>449</v>
-      </c>
-      <c r="M1" t="s">
-        <v>450</v>
-      </c>
-      <c r="N1" t="s">
-        <v>451</v>
-      </c>
-      <c r="O1" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" t="s">
         <v>453</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="6" t="s">
         <v>454</v>
-      </c>
-      <c r="C2" t="s">
-        <v>455</v>
-      </c>
-      <c r="D2" t="s">
-        <v>456</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>457</v>
       </c>
       <c r="F2" t="str">
         <f>LOWER(G2)</f>
@@ -7155,7 +7374,7 @@
         <v>internal</v>
       </c>
       <c r="I2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J2" t="str">
         <f>LOWER(K2)</f>
@@ -7165,17 +7384,17 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="M2" t="str">
         <f>LOWER(N2)</f>
         <v>implanted</v>
       </c>
       <c r="N2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -7213,86 +7432,86 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1" t="s">
         <v>438</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>459</v>
+      </c>
+      <c r="F1" t="s">
         <v>439</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>440</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>441</v>
       </c>
-      <c r="E1" t="s">
-        <v>462</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>442</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>443</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>444</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>445</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>446</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>447</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>448</v>
       </c>
-      <c r="M1" t="s">
-        <v>449</v>
-      </c>
-      <c r="N1" t="s">
-        <v>450</v>
-      </c>
-      <c r="O1" t="s">
-        <v>451</v>
-      </c>
       <c r="P1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B2" t="s">
+        <v>461</v>
+      </c>
+      <c r="C2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" t="s">
+        <v>462</v>
+      </c>
+      <c r="E2" t="s">
+        <v>463</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>464</v>
-      </c>
-      <c r="C2" t="s">
-        <v>455</v>
-      </c>
-      <c r="D2" t="s">
-        <v>465</v>
-      </c>
-      <c r="E2" t="s">
-        <v>466</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>467</v>
       </c>
       <c r="G2" t="str">
         <f>SUBSTITUTE(LOWER(H2)," ","")</f>
         <v>firststage</v>
       </c>
       <c r="H2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I2" t="str">
         <f>LOWER(J2)</f>
         <v>external</v>
       </c>
       <c r="J2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="K2" t="str">
         <f>LOWER(L2)</f>
@@ -7302,7 +7521,7 @@
         <v>184</v>
       </c>
       <c r="M2" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="N2" t="str">
         <f>LOWER(O2)</f>
@@ -7312,7 +7531,7 @@
         <v>205</v>
       </c>
       <c r="P2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -7345,126 +7564,126 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1" t="s">
         <v>472</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>473</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>474</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>475</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>476</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>477</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>478</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>479</v>
-      </c>
-      <c r="I1" t="s">
-        <v>480</v>
-      </c>
-      <c r="J1" t="s">
-        <v>481</v>
-      </c>
-      <c r="K1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C2" t="s">
+        <v>482</v>
+      </c>
+      <c r="D2" t="s">
         <v>483</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>484</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>485</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>486</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
         <v>487</v>
-      </c>
-      <c r="F2" t="s">
-        <v>488</v>
-      </c>
-      <c r="G2" t="s">
-        <v>489</v>
-      </c>
-      <c r="K2" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B3" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D3" t="s">
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>492</v>
+      </c>
+      <c r="B4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C4" t="s">
+        <v>494</v>
+      </c>
+      <c r="D4" t="s">
         <v>495</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>496</v>
       </c>
-      <c r="C4" t="s">
+      <c r="K4" t="s">
         <v>497</v>
-      </c>
-      <c r="D4" t="s">
-        <v>498</v>
-      </c>
-      <c r="E4" t="s">
-        <v>499</v>
-      </c>
-      <c r="K4" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>498</v>
+      </c>
+      <c r="B5" t="s">
+        <v>499</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="D5" t="s">
         <v>501</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>502</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="D5" t="s">
-        <v>504</v>
-      </c>
-      <c r="E5" t="s">
-        <v>505</v>
-      </c>
       <c r="F5" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G5" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="H5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="I5" t="s">
         <v>100</v>
@@ -7473,7 +7692,7 @@
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7513,43 +7732,43 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1" t="s">
         <v>472</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>473</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>474</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>475</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>476</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>477</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>478</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>479</v>
       </c>
-      <c r="I1" t="s">
-        <v>480</v>
-      </c>
-      <c r="J1" t="s">
-        <v>481</v>
-      </c>
-      <c r="K1" t="s">
-        <v>482</v>
-      </c>
       <c r="L1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="M1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="N1" t="s">
         <v>122</v>
@@ -7557,118 +7776,118 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C2" t="s">
+        <v>507</v>
+      </c>
+      <c r="D2" t="s">
+        <v>508</v>
+      </c>
+      <c r="E2" t="s">
         <v>509</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>510</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>511</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
         <v>512</v>
       </c>
-      <c r="F2" t="s">
+      <c r="L2" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="G2" t="s">
+      <c r="M2" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="N2" t="s">
         <v>514</v>
-      </c>
-      <c r="K2" t="s">
-        <v>515</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="N2" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B3" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="N3" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B4" t="s">
+        <v>518</v>
+      </c>
+      <c r="C4" t="s">
+        <v>519</v>
+      </c>
+      <c r="D4" t="s">
+        <v>520</v>
+      </c>
+      <c r="E4" t="s">
         <v>521</v>
       </c>
-      <c r="C4" t="s">
+      <c r="K4" t="s">
         <v>522</v>
       </c>
-      <c r="D4" t="s">
-        <v>523</v>
-      </c>
-      <c r="E4" t="s">
-        <v>524</v>
-      </c>
-      <c r="K4" t="s">
-        <v>525</v>
-      </c>
       <c r="L4" s="5" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="N4" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>498</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="C5" t="s">
         <v>501</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="C5" t="s">
-        <v>504</v>
-      </c>
       <c r="D5" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F5" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="G5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="H5" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="I5" t="s">
         <v>60</v>
@@ -7677,16 +7896,16 @@
         <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="N5" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -7729,160 +7948,160 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E1" t="s">
         <v>527</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>528</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>529</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>530</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>531</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>532</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>533</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>534</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>535</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>536</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>537</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>538</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>539</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>540</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>541</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>542</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>543</v>
-      </c>
-      <c r="S1" t="s">
-        <v>544</v>
-      </c>
-      <c r="T1" t="s">
-        <v>545</v>
-      </c>
-      <c r="U1" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>544</v>
+      </c>
+      <c r="B2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C2" t="s">
+        <v>546</v>
+      </c>
+      <c r="D2" t="s">
         <v>547</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>548</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>549</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>550</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>551</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>552</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>553</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>554</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>555</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>556</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>557</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>558</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>559</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>560</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>561</v>
       </c>
-      <c r="Q2" t="s">
-        <v>562</v>
-      </c>
-      <c r="R2" t="s">
-        <v>563</v>
-      </c>
-      <c r="S2" t="s">
-        <v>564</v>
-      </c>
       <c r="U2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C3" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="D3" t="s">
         <v>316</v>
       </c>
       <c r="O3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="T3" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="U3" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>568</v>
+      </c>
+      <c r="O4" t="s">
+        <v>569</v>
+      </c>
+      <c r="T4" t="s">
+        <v>570</v>
+      </c>
+      <c r="U4" t="s">
         <v>571</v>
-      </c>
-      <c r="O4" t="s">
-        <v>572</v>
-      </c>
-      <c r="T4" t="s">
-        <v>573</v>
-      </c>
-      <c r="U4" t="s">
-        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -7928,70 +8147,70 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E1" t="s">
         <v>527</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>528</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>529</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>530</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>531</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>532</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>533</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>534</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>535</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>536</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>537</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>538</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>539</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>540</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>541</v>
       </c>
-      <c r="Q1" t="s">
-        <v>542</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>543</v>
-      </c>
-      <c r="S1" t="s">
-        <v>544</v>
-      </c>
-      <c r="T1" t="s">
-        <v>546</v>
       </c>
       <c r="U1" t="s">
         <v>132</v>
       </c>
       <c r="V1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="W1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="X1" t="s">
         <v>122</v>
@@ -7999,93 +8218,93 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C2" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2" t="s">
+        <v>574</v>
+      </c>
+      <c r="E2" t="s">
+        <v>575</v>
+      </c>
+      <c r="F2" t="s">
+        <v>545</v>
+      </c>
+      <c r="G2" t="s">
+        <v>546</v>
+      </c>
+      <c r="H2" t="s">
+        <v>576</v>
+      </c>
+      <c r="I2" t="s">
+        <v>555</v>
+      </c>
+      <c r="J2" t="s">
+        <v>556</v>
+      </c>
+      <c r="K2" t="s">
+        <v>577</v>
+      </c>
+      <c r="L2" t="s">
         <v>552</v>
       </c>
-      <c r="C2" t="s">
+      <c r="M2" t="s">
         <v>553</v>
       </c>
-      <c r="D2" t="s">
-        <v>577</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="N2" t="s">
         <v>578</v>
       </c>
-      <c r="F2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="P2" t="s">
         <v>579</v>
       </c>
-      <c r="I2" t="s">
-        <v>558</v>
-      </c>
-      <c r="J2" t="s">
-        <v>559</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="Q2" t="s">
         <v>580</v>
       </c>
-      <c r="L2" t="s">
-        <v>555</v>
-      </c>
-      <c r="M2" t="s">
-        <v>556</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>581</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>582</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
+        <v>544</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>583</v>
       </c>
-      <c r="R2" t="s">
+      <c r="V2" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="X2" t="s">
         <v>584</v>
-      </c>
-      <c r="S2" t="s">
-        <v>585</v>
-      </c>
-      <c r="T2" t="s">
-        <v>547</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>586</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>586</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>586</v>
-      </c>
-      <c r="X2" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>186</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -8096,45 +8315,45 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="T3" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="X3" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>568</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="O4" t="s">
+        <v>592</v>
+      </c>
+      <c r="T4" t="s">
         <v>571</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>593</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>594</v>
-      </c>
-      <c r="O4" t="s">
-        <v>595</v>
-      </c>
-      <c r="T4" t="s">
-        <v>574</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>596</v>
-      </c>
       <c r="W4" s="5" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="X4" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -8176,108 +8395,108 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C1" t="s">
+        <v>596</v>
+      </c>
+      <c r="D1" t="s">
         <v>597</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>598</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>599</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>600</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>601</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>602</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>603</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>604</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>605</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>606</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>607</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>608</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>609</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>610</v>
-      </c>
-      <c r="O1" t="s">
-        <v>611</v>
-      </c>
-      <c r="P1" t="s">
-        <v>612</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>611</v>
+      </c>
+      <c r="B2" t="s">
+        <v>612</v>
+      </c>
+      <c r="C2" t="s">
+        <v>613</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>614</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="6" t="s">
         <v>615</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>616</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="G2" t="s">
         <v>617</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="H2" t="s">
         <v>618</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>619</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>620</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>621</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>622</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>623</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>624</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>625</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>626</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" s="10" t="s">
         <v>627</v>
-      </c>
-      <c r="O2" t="s">
-        <v>628</v>
-      </c>
-      <c r="P2" t="s">
-        <v>629</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -8331,121 +8550,121 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C1" t="s">
+        <v>628</v>
+      </c>
+      <c r="D1" t="s">
+        <v>596</v>
+      </c>
+      <c r="E1" t="s">
         <v>597</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>598</v>
       </c>
-      <c r="C1" t="s">
-        <v>631</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>629</v>
+      </c>
+      <c r="H1" t="s">
         <v>599</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>600</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>601</v>
       </c>
-      <c r="G1" t="s">
-        <v>632</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>602</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>603</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>604</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>605</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>606</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>607</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>608</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>609</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>610</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>611</v>
-      </c>
-      <c r="R1" t="s">
-        <v>612</v>
-      </c>
-      <c r="S1" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C2" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D2" t="str">
         <f>LOWER(C2)</f>
         <v>withdrawn</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="H2" t="s">
+        <v>616</v>
+      </c>
+      <c r="I2" t="s">
         <v>617</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="H2" t="s">
-        <v>619</v>
-      </c>
-      <c r="I2" t="s">
-        <v>620</v>
-      </c>
       <c r="J2" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="K2" t="s">
+        <v>631</v>
+      </c>
+      <c r="L2" t="s">
+        <v>632</v>
+      </c>
+      <c r="M2" t="s">
+        <v>633</v>
+      </c>
+      <c r="N2" t="s">
         <v>634</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>635</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>636</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>637</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>638</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" s="10" t="s">
         <v>639</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>640</v>
-      </c>
-      <c r="R2" t="s">
-        <v>641</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -8469,47 +8688,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B1" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>82</v>
@@ -8517,143 +8736,143 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>316</v>
@@ -8661,26 +8880,26 @@
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -8837,6 +9056,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9091,27 +9330,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9128,23 +9366,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Push All required change with worklist pathway and tasks
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B3E11A-AD6B-4BD1-A8D1-3C45E55C3A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7424F265-E4CF-4417-BF15-8EA366A64957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,22 +68,23 @@
     <sheet name="EditPatientDetails" sheetId="53" r:id="rId53"/>
     <sheet name="DeletePatientDetails" sheetId="54" r:id="rId54"/>
     <sheet name="AddTask" sheetId="55" r:id="rId55"/>
-    <sheet name="EditTask" sheetId="56" r:id="rId56"/>
-    <sheet name="AddCarePlan" sheetId="57" r:id="rId57"/>
-    <sheet name="EditCarePlan" sheetId="58" r:id="rId58"/>
-    <sheet name="DeleteCarePlan" sheetId="59" r:id="rId59"/>
-    <sheet name="Alerts" sheetId="60" r:id="rId60"/>
-    <sheet name="DeleteInvestigation" sheetId="62" r:id="rId61"/>
-    <sheet name="DevicePatientDetails" sheetId="63" r:id="rId62"/>
-    <sheet name="AddDevice" sheetId="64" r:id="rId63"/>
-    <sheet name="EditDevice" sheetId="65" r:id="rId64"/>
-    <sheet name="AddTest" sheetId="66" r:id="rId65"/>
-    <sheet name="EditTest" sheetId="67" r:id="rId66"/>
-    <sheet name="AddTool" sheetId="68" r:id="rId67"/>
-    <sheet name="EditTool" sheetId="69" r:id="rId68"/>
-    <sheet name="AddPatientConsent" sheetId="70" r:id="rId69"/>
-    <sheet name="EditPatientConsent" sheetId="71" r:id="rId70"/>
-    <sheet name="PhysicalSign" sheetId="72" r:id="rId71"/>
+    <sheet name="AddWorklist" sheetId="73" r:id="rId56"/>
+    <sheet name="EditTask" sheetId="56" r:id="rId57"/>
+    <sheet name="AddCarePlan" sheetId="57" r:id="rId58"/>
+    <sheet name="EditCarePlan" sheetId="58" r:id="rId59"/>
+    <sheet name="DeleteCarePlan" sheetId="59" r:id="rId60"/>
+    <sheet name="Alerts" sheetId="60" r:id="rId61"/>
+    <sheet name="DeleteInvestigation" sheetId="62" r:id="rId62"/>
+    <sheet name="DevicePatientDetails" sheetId="63" r:id="rId63"/>
+    <sheet name="AddDevice" sheetId="64" r:id="rId64"/>
+    <sheet name="EditDevice" sheetId="65" r:id="rId65"/>
+    <sheet name="AddTest" sheetId="66" r:id="rId66"/>
+    <sheet name="EditTest" sheetId="67" r:id="rId67"/>
+    <sheet name="AddTool" sheetId="68" r:id="rId68"/>
+    <sheet name="EditTool" sheetId="69" r:id="rId69"/>
+    <sheet name="AddPatientConsent" sheetId="70" r:id="rId70"/>
+    <sheet name="EditPatientConsent" sheetId="71" r:id="rId71"/>
+    <sheet name="PhysicalSign" sheetId="72" r:id="rId72"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="727">
   <si>
     <t>username</t>
   </si>
@@ -2265,16 +2266,28 @@
     <t>Review</t>
   </si>
   <si>
-    <t>Prerelease</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>hosp2560</t>
-  </si>
-  <si>
-    <t>01-01-1999</t>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>wor_name</t>
+  </si>
+  <si>
+    <t>wor_rename</t>
+  </si>
+  <si>
+    <t>Book New Appointment</t>
+  </si>
+  <si>
+    <t>10-10-2024</t>
+  </si>
+  <si>
+    <t>20-10-2024</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
   </si>
 </sst>
 </file>
@@ -2334,7 +2347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2364,9 +2377,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3354,10 +3364,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF0DF87-67F2-4E87-A7EE-C4365800D834}">
-  <dimension ref="A1:AV8"/>
+  <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3516,22 +3526,22 @@
     </row>
     <row r="2" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>721</v>
+        <v>699</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>720</v>
+        <v>430</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>719</v>
+        <v>698</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>302</v>
+        <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>722</v>
+      <c r="I2" s="16" t="s">
+        <v>697</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>51</v>
@@ -3600,95 +3610,6 @@
         <v>65</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
-        <v>699</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>698</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>697</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="W8" s="2">
-        <v>0</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AV8" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3924,7 +3845,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>28/10/2025</v>
+        <v>30/10/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -4003,7 +3924,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>28/10/2025</v>
+        <v>30/10/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -4249,7 +4170,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45958</v>
+        <v>45960</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>102</v>
@@ -6499,7 +6420,7 @@
       </c>
       <c r="H2" s="9" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>28/10/2025</v>
+        <v>30/10/2025</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>350</v>
@@ -6547,11 +6468,99 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5764F40-426A-43BC-8A50-6EAFA8D7F160}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E1" t="s">
+        <v>721</v>
+      </c>
+      <c r="F1" t="s">
+        <v>722</v>
+      </c>
+      <c r="G1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I1" t="s">
+        <v>346</v>
+      </c>
+      <c r="J1" t="s">
+        <v>347</v>
+      </c>
+      <c r="K1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" t="s">
+        <v>723</v>
+      </c>
+      <c r="F2" t="s">
+        <v>723</v>
+      </c>
+      <c r="G2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="K2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B730A7AF-1268-4970-A808-63C4CFDE9D42}">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6649,7 +6658,7 @@
       </c>
       <c r="H2" s="9" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>28/10/2025</v>
+        <v>30/10/2025</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>717</v>
@@ -6687,7 +6696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCFF350-CD6D-4EA3-AD07-F7835D15A2E0}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -6814,7 +6823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019DB1EE-87BC-46CC-8969-22DDA41D9703}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -6941,18 +6950,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073EB301-EA84-4595-9FAF-2D4DB18F33CC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3765FB4-F532-4FCF-A614-4266393F4C44}">
   <dimension ref="A1:C2"/>
@@ -6997,6 +6994,18 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073EB301-EA84-4595-9FAF-2D4DB18F33CC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292FBDAE-D596-4C82-A946-FDA545BEF94C}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -7063,7 +7072,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>28/10/2025</v>
+        <v>30/10/2025</v>
       </c>
       <c r="C2" t="s">
         <v>409</v>
@@ -7098,7 +7107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9C9D7F-0AE8-4EC3-92AB-0B4F9C52B57D}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -7226,7 +7235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AFB2BB-3003-4319-BBC1-012DC5CD548F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -7275,7 +7284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251B21E0-6337-4D24-89BA-CCC72B4CE178}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -7405,7 +7414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46978773-1075-4167-9B69-BED932E2DB61}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -7542,7 +7551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DAE407-BA0B-4688-BBAD-7DFB774DB5BC}">
   <dimension ref="A1:K7"/>
   <sheetViews>
@@ -7709,7 +7718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8677F37-19B8-4D20-9C0F-A78F8917B3F1}">
   <dimension ref="A1:N5"/>
   <sheetViews>
@@ -7916,7 +7925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BEBF31-D55A-4984-AA77-9D15D13575B6}">
   <dimension ref="A1:U4"/>
   <sheetViews>
@@ -8112,7 +8121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8312F661-F5B3-473F-B72C-C78A4DEC965C}">
   <dimension ref="A1:X5"/>
   <sheetViews>
@@ -8368,7 +8377,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3310FF1D-4559-4E35-BB7B-0285AF82C887}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC60C30C-7F9A-433E-9C84-B91C8DACEF30}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -8507,22 +8531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3310FF1D-4559-4E35-BB7B-0285AF82C887}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC450EAE-2668-49BB-BB00-38055CC0A139}">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -8675,7 +8684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847F356E-F54A-4994-9714-D3DDDBAEB896}">
   <dimension ref="A1:B27"/>
   <sheetViews>
@@ -9059,26 +9068,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9333,26 +9322,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9369,4 +9359,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DB change to linux
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7424F265-E4CF-4417-BF15-8EA366A64957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E355A3E5-74B2-4651-BABF-2024A75A566F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3367,7 +3367,7 @@
   <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9068,6 +9068,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9322,7 +9331,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
@@ -9333,16 +9342,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9361,7 +9369,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9370,12 +9378,4 @@
     <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
in social change Diet to Dietitian
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981F0841-F6D3-465C-8B75-8F2C8F8189DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BAF12C-C7CE-4D83-9A50-EB718362EE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="25" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="34" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -892,9 +892,6 @@
     <t>Overview Edited</t>
   </si>
   <si>
-    <t>Diet</t>
-  </si>
-  <si>
     <t>Added Notes for Social Circumstances</t>
   </si>
   <si>
@@ -2291,6 +2288,9 @@
   </si>
   <si>
     <t>Division of Left Knee Tendon, Open Approach</t>
+  </si>
+  <si>
+    <t>Dietitian</t>
   </si>
 </sst>
 </file>
@@ -2685,34 +2685,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>700</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -3208,16 +3208,16 @@
         <v>159</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>157</v>
       </c>
       <c r="L2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M2" t="s">
         <v>188</v>
@@ -3529,22 +3529,22 @@
     </row>
     <row r="2" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>51</v>
@@ -3664,7 +3664,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" t="s">
         <v>131</v>
@@ -3727,7 +3727,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" t="s">
         <v>116</v>
@@ -3778,7 +3778,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>10/11/2025</v>
+        <v>11/11/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -3857,10 +3857,10 @@
         <v>194</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>281</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>282</v>
       </c>
       <c r="I2" s="7"/>
     </row>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>10/11/2025</v>
+        <v>11/11/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -3936,10 +3936,10 @@
         <v>194</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3993,7 +3993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AC72BC-1449-4578-8E57-945920649F3D}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4062,19 +4062,19 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>102</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>214</v>
@@ -4169,17 +4169,17 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>102</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>214</v>
@@ -4239,7 +4239,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -4572,7 +4572,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4584,7 +4584,7 @@
         <v>247</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G2" t="s">
         <v>248</v>
@@ -4670,7 +4670,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4729,7 +4729,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B2" t="s">
         <v>255</v>
@@ -4892,7 +4892,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4911,7 +4911,7 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D1" t="s">
         <v>126</v>
@@ -4919,16 +4919,16 @@
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
+        <v>727</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" t="s">
         <v>262</v>
-      </c>
-      <c r="D2" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -4941,7 +4941,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4960,7 +4960,7 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D1" t="s">
         <v>126</v>
@@ -4968,16 +4968,16 @@
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>727</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -5037,7 +5037,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -5127,7 +5127,7 @@
         <v>200</v>
       </c>
       <c r="AH1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -5135,13 +5135,13 @@
         <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E2" t="s">
         <v>71</v>
@@ -5159,10 +5159,10 @@
         <v>102</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>639</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>640</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>641</v>
       </c>
       <c r="L2" t="s">
         <v>176</v>
@@ -5195,7 +5195,7 @@
         <v>82</v>
       </c>
       <c r="X2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Y2" t="s">
         <v>104</v>
@@ -5225,7 +5225,7 @@
         <v>201</v>
       </c>
       <c r="AH2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -5237,8 +5237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF82F3D0-82CD-49AF-BA0A-7CEE53FBA6AC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5261,10 +5261,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>727</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -5299,7 +5299,7 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D1" t="s">
         <v>126</v>
@@ -5307,16 +5307,16 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -5348,7 +5348,7 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D1" t="s">
         <v>126</v>
@@ -5356,16 +5356,16 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>700</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="D2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -5401,13 +5401,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -5438,7 +5438,7 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D1" t="s">
         <v>126</v>
@@ -5446,16 +5446,16 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -5486,7 +5486,7 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D1" t="s">
         <v>126</v>
@@ -5494,16 +5494,16 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B2" t="s">
-        <v>366</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>277</v>
-      </c>
       <c r="D2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -5539,13 +5539,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -5580,69 +5580,69 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D1" t="s">
         <v>126</v>
       </c>
       <c r="E1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" t="s">
         <v>288</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>289</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>290</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>291</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>292</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>293</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>294</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>295</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>296</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>297</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>298</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>299</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" t="s">
         <v>284</v>
-      </c>
-      <c r="B2" t="s">
-        <v>285</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H2" t="s">
         <v>131</v>
@@ -5651,28 +5651,28 @@
         <v>100</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K2" t="s">
         <v>98</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="O2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -5708,81 +5708,81 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D1" t="s">
         <v>126</v>
       </c>
       <c r="E1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" t="s">
         <v>288</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>289</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>290</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>291</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>292</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>293</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>294</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>295</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>296</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>297</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>298</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>299</v>
       </c>
-      <c r="Q1" t="s">
-        <v>300</v>
-      </c>
       <c r="R1" t="s">
+        <v>312</v>
+      </c>
+      <c r="S1" t="s">
         <v>313</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>314</v>
       </c>
-      <c r="T1" t="s">
-        <v>315</v>
-      </c>
       <c r="U1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" t="s">
         <v>284</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2" t="s">
         <v>285</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G2" t="s">
         <v>310</v>
-      </c>
-      <c r="D2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G2" t="s">
-        <v>311</v>
       </c>
       <c r="H2" t="s">
         <v>131</v>
@@ -5791,40 +5791,40 @@
         <v>100</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K2" t="s">
         <v>98</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="O2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R2" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>317</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -5857,13 +5857,13 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D1" t="s">
         <v>132</v>
       </c>
       <c r="E1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" t="s">
         <v>126</v>
@@ -5871,22 +5871,22 @@
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>642</v>
       </c>
-      <c r="B2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>644</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>643</v>
-      </c>
       <c r="E2" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" t="s">
         <v>325</v>
-      </c>
-      <c r="F2" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -5935,7 +5935,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -6007,7 +6007,7 @@
         <v>112</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E2" t="s">
         <v>86</v>
@@ -6091,13 +6091,13 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D1" t="s">
         <v>132</v>
       </c>
       <c r="E1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" t="s">
         <v>126</v>
@@ -6105,22 +6105,22 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" t="s">
         <v>321</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>324</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -6155,13 +6155,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" t="s">
         <v>321</v>
       </c>
-      <c r="B2" t="s">
-        <v>322</v>
-      </c>
       <c r="C2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -6196,21 +6196,21 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>330</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>331</v>
-      </c>
-      <c r="D2" t="s">
-        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -6246,21 +6246,21 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>330</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>331</v>
-      </c>
-      <c r="D2" t="s">
-        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -6296,13 +6296,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>330</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -6336,67 +6336,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B1" t="s">
         <v>703</v>
       </c>
-      <c r="B1" t="s">
-        <v>704</v>
-      </c>
       <c r="C1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E1" t="s">
+        <v>709</v>
+      </c>
+      <c r="F1" t="s">
         <v>710</v>
       </c>
-      <c r="F1" t="s">
-        <v>711</v>
-      </c>
       <c r="G1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H1" t="s">
         <v>334</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>335</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>336</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>337</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>338</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>339</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>340</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>341</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>342</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>343</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>344</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>345</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>346</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>347</v>
-      </c>
-      <c r="U1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -6404,65 +6404,65 @@
         <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H2" s="9" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>10/11/2025</v>
+        <v>11/11/2025</v>
       </c>
       <c r="I2" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" t="s">
         <v>352</v>
       </c>
-      <c r="L2" t="s">
-        <v>353</v>
-      </c>
       <c r="M2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N2" t="s">
         <v>98</v>
       </c>
       <c r="O2" t="s">
+        <v>353</v>
+      </c>
+      <c r="P2" t="s">
         <v>354</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>355</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>356</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" t="s">
         <v>358</v>
-      </c>
-      <c r="U2" t="s">
-        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -6485,72 +6485,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>717</v>
+      </c>
+      <c r="B1" t="s">
         <v>718</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E1" t="s">
         <v>719</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>720</v>
+      </c>
+      <c r="G1" t="s">
         <v>361</v>
       </c>
-      <c r="D1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E1" t="s">
-        <v>720</v>
-      </c>
-      <c r="F1" t="s">
-        <v>721</v>
-      </c>
-      <c r="G1" t="s">
-        <v>362</v>
-      </c>
       <c r="H1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I1" t="s">
+        <v>345</v>
+      </c>
+      <c r="J1" t="s">
         <v>346</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>347</v>
-      </c>
-      <c r="K1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>723</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="12" t="s">
         <v>724</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>725</v>
-      </c>
       <c r="D2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="K2" t="s">
         <v>358</v>
-      </c>
-      <c r="K2" t="s">
-        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -6583,58 +6583,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B1" t="s">
         <v>703</v>
       </c>
-      <c r="B1" t="s">
-        <v>704</v>
-      </c>
       <c r="C1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E1" t="s">
+        <v>709</v>
+      </c>
+      <c r="F1" t="s">
         <v>710</v>
       </c>
-      <c r="F1" t="s">
-        <v>711</v>
-      </c>
       <c r="G1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H1" t="s">
+        <v>359</v>
+      </c>
+      <c r="I1" t="s">
         <v>360</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K1" t="s">
+        <v>339</v>
+      </c>
+      <c r="L1" t="s">
+        <v>340</v>
+      </c>
+      <c r="M1" t="s">
+        <v>341</v>
+      </c>
+      <c r="N1" t="s">
         <v>361</v>
       </c>
-      <c r="J1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K1" t="s">
-        <v>340</v>
-      </c>
-      <c r="L1" t="s">
-        <v>341</v>
-      </c>
-      <c r="M1" t="s">
-        <v>342</v>
-      </c>
-      <c r="N1" t="s">
-        <v>362</v>
-      </c>
       <c r="O1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P1" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q1" t="s">
         <v>346</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>347</v>
-      </c>
-      <c r="R1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -6642,56 +6642,56 @@
         <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D2" t="s">
+        <v>713</v>
+      </c>
+      <c r="E2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="E2" t="s">
-        <v>713</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>715</v>
-      </c>
       <c r="G2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H2" s="9" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>10/11/2025</v>
+        <v>11/11/2025</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="J2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L2" t="s">
         <v>98</v>
       </c>
       <c r="M2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q2" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="R2" t="s">
         <v>358</v>
-      </c>
-      <c r="R2" t="s">
-        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -6732,93 +6732,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" t="s">
         <v>372</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>373</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>374</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>375</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>376</v>
       </c>
-      <c r="H1" t="s">
-        <v>377</v>
-      </c>
       <c r="I1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N1" t="s">
+        <v>393</v>
+      </c>
+      <c r="O1" t="s">
         <v>394</v>
-      </c>
-      <c r="O1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F2" t="s">
+        <v>380</v>
+      </c>
+      <c r="G2" t="s">
+        <v>381</v>
+      </c>
+      <c r="H2" t="s">
+        <v>382</v>
+      </c>
+      <c r="I2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J2" t="s">
+        <v>386</v>
+      </c>
+      <c r="K2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L2" t="s">
+        <v>390</v>
+      </c>
+      <c r="M2" t="s">
+        <v>392</v>
+      </c>
+      <c r="N2" t="s">
         <v>397</v>
       </c>
-      <c r="B2" t="s">
-        <v>371</v>
-      </c>
-      <c r="C2" t="s">
-        <v>378</v>
-      </c>
-      <c r="D2" t="s">
-        <v>379</v>
-      </c>
-      <c r="E2" t="s">
-        <v>380</v>
-      </c>
-      <c r="F2" t="s">
-        <v>381</v>
-      </c>
-      <c r="G2" t="s">
-        <v>382</v>
-      </c>
-      <c r="H2" t="s">
-        <v>383</v>
-      </c>
-      <c r="I2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J2" t="s">
-        <v>387</v>
-      </c>
-      <c r="K2" t="s">
-        <v>389</v>
-      </c>
-      <c r="L2" t="s">
-        <v>391</v>
-      </c>
-      <c r="M2" t="s">
-        <v>393</v>
-      </c>
-      <c r="N2" t="s">
-        <v>398</v>
-      </c>
       <c r="O2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="P2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -6859,93 +6859,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" t="s">
         <v>372</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>373</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>374</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>375</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>376</v>
       </c>
-      <c r="H1" t="s">
-        <v>377</v>
-      </c>
       <c r="I1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N1" t="s">
+        <v>393</v>
+      </c>
+      <c r="O1" t="s">
         <v>394</v>
-      </c>
-      <c r="O1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D2" t="s">
         <v>378</v>
       </c>
-      <c r="D2" t="s">
-        <v>379</v>
-      </c>
       <c r="E2" t="s">
+        <v>398</v>
+      </c>
+      <c r="F2" t="s">
+        <v>380</v>
+      </c>
+      <c r="G2" t="s">
+        <v>381</v>
+      </c>
+      <c r="H2" t="s">
         <v>399</v>
       </c>
-      <c r="F2" t="s">
-        <v>381</v>
-      </c>
-      <c r="G2" t="s">
-        <v>382</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J2" t="s">
+        <v>386</v>
+      </c>
+      <c r="K2" t="s">
         <v>400</v>
       </c>
-      <c r="I2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J2" t="s">
-        <v>387</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>390</v>
+      </c>
+      <c r="M2" t="s">
+        <v>392</v>
+      </c>
+      <c r="N2" t="s">
         <v>401</v>
       </c>
-      <c r="L2" t="s">
-        <v>391</v>
-      </c>
-      <c r="M2" t="s">
-        <v>393</v>
-      </c>
-      <c r="N2" t="s">
-        <v>402</v>
-      </c>
       <c r="O2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="P2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -7033,76 +7033,76 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B1" t="s">
         <v>403</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>404</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>405</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>406</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>407</v>
       </c>
-      <c r="F1" t="s">
-        <v>408</v>
-      </c>
       <c r="G1" t="s">
+        <v>410</v>
+      </c>
+      <c r="H1" t="s">
         <v>411</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>412</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>413</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>414</v>
       </c>
-      <c r="K1" t="s">
-        <v>415</v>
-      </c>
       <c r="L1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>10/11/2025</v>
+        <v>11/11/2025</v>
       </c>
       <c r="C2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D2" t="s">
         <v>409</v>
       </c>
-      <c r="D2" t="s">
-        <v>410</v>
-      </c>
       <c r="E2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F2" t="s">
         <v>116</v>
       </c>
       <c r="H2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I2" t="s">
         <v>416</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>417</v>
       </c>
-      <c r="J2" t="s">
-        <v>418</v>
-      </c>
       <c r="K2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -7143,63 +7143,63 @@
         <v>126</v>
       </c>
       <c r="E1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" t="s">
         <v>288</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>289</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>290</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>291</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>292</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>293</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>294</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>295</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>296</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>297</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>298</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>299</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" t="s">
         <v>284</v>
-      </c>
-      <c r="B2" t="s">
-        <v>285</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>255</v>
       </c>
       <c r="D2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H2" t="s">
         <v>131</v>
@@ -7208,28 +7208,28 @@
         <v>100</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K2" t="s">
         <v>98</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -7270,16 +7270,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>432</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -7316,66 +7316,66 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" t="s">
         <v>434</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>435</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>436</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>437</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>438</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>439</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>440</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>441</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>442</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>443</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>444</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>445</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>446</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>447</v>
-      </c>
-      <c r="O1" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B2" t="s">
         <v>449</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>450</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>451</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="6" t="s">
         <v>452</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>453</v>
       </c>
       <c r="F2" t="str">
         <f>LOWER(G2)</f>
@@ -7389,7 +7389,7 @@
         <v>internal</v>
       </c>
       <c r="I2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J2" t="str">
         <f>LOWER(K2)</f>
@@ -7399,17 +7399,17 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="M2" t="str">
         <f>LOWER(N2)</f>
         <v>implanted</v>
       </c>
       <c r="N2" t="s">
+        <v>455</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>456</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -7447,86 +7447,86 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" t="s">
         <v>434</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>435</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>436</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F1" t="s">
         <v>437</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H1" t="s">
+        <v>439</v>
+      </c>
+      <c r="I1" t="s">
+        <v>440</v>
+      </c>
+      <c r="J1" t="s">
+        <v>441</v>
+      </c>
+      <c r="K1" t="s">
+        <v>442</v>
+      </c>
+      <c r="L1" t="s">
+        <v>443</v>
+      </c>
+      <c r="M1" t="s">
+        <v>444</v>
+      </c>
+      <c r="N1" t="s">
+        <v>445</v>
+      </c>
+      <c r="O1" t="s">
+        <v>446</v>
+      </c>
+      <c r="P1" t="s">
         <v>458</v>
-      </c>
-      <c r="F1" t="s">
-        <v>438</v>
-      </c>
-      <c r="G1" t="s">
-        <v>439</v>
-      </c>
-      <c r="H1" t="s">
-        <v>440</v>
-      </c>
-      <c r="I1" t="s">
-        <v>441</v>
-      </c>
-      <c r="J1" t="s">
-        <v>442</v>
-      </c>
-      <c r="K1" t="s">
-        <v>443</v>
-      </c>
-      <c r="L1" t="s">
-        <v>444</v>
-      </c>
-      <c r="M1" t="s">
-        <v>445</v>
-      </c>
-      <c r="N1" t="s">
-        <v>446</v>
-      </c>
-      <c r="O1" t="s">
-        <v>447</v>
-      </c>
-      <c r="P1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D2" t="s">
         <v>460</v>
       </c>
-      <c r="C2" t="s">
-        <v>451</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>461</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="6" t="s">
         <v>462</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>463</v>
       </c>
       <c r="G2" t="str">
         <f>SUBSTITUTE(LOWER(H2)," ","")</f>
         <v>firststage</v>
       </c>
       <c r="H2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I2" t="str">
         <f>LOWER(J2)</f>
         <v>external</v>
       </c>
       <c r="J2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K2" t="str">
         <f>LOWER(L2)</f>
@@ -7536,7 +7536,7 @@
         <v>184</v>
       </c>
       <c r="M2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="N2" t="str">
         <f>LOWER(O2)</f>
@@ -7546,7 +7546,7 @@
         <v>205</v>
       </c>
       <c r="P2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -7579,126 +7579,126 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B1" t="s">
         <v>468</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>469</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>470</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>471</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>472</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>473</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>474</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>475</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>476</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>477</v>
-      </c>
-      <c r="K1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B2" t="s">
         <v>479</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>480</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>481</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>482</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>483</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>484</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>485</v>
-      </c>
-      <c r="K2" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B3" t="s">
         <v>487</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>488</v>
-      </c>
-      <c r="C3" t="s">
-        <v>489</v>
       </c>
       <c r="D3" t="s">
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B4" t="s">
         <v>491</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>492</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>493</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>494</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>495</v>
-      </c>
-      <c r="K4" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>496</v>
+      </c>
+      <c r="B5" t="s">
         <v>497</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" t="s">
         <v>499</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>500</v>
       </c>
-      <c r="E5" t="s">
-        <v>501</v>
-      </c>
       <c r="F5" t="s">
+        <v>497</v>
+      </c>
+      <c r="G5" t="s">
         <v>498</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>499</v>
-      </c>
-      <c r="H5" t="s">
-        <v>500</v>
       </c>
       <c r="I5" t="s">
         <v>100</v>
@@ -7707,7 +7707,7 @@
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7747,43 +7747,43 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B1" t="s">
         <v>468</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>469</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>470</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>471</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>472</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>473</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>474</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>475</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>476</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>477</v>
       </c>
-      <c r="K1" t="s">
-        <v>478</v>
-      </c>
       <c r="L1" t="s">
+        <v>502</v>
+      </c>
+      <c r="M1" t="s">
         <v>503</v>
-      </c>
-      <c r="M1" t="s">
-        <v>504</v>
       </c>
       <c r="N1" t="s">
         <v>122</v>
@@ -7791,118 +7791,118 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C2" t="s">
         <v>505</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>506</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>507</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>508</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>509</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>510</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="N2" t="s">
         <v>512</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="N2" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B3" t="s">
+        <v>513</v>
+      </c>
+      <c r="C3" t="s">
         <v>514</v>
-      </c>
-      <c r="C3" t="s">
-        <v>515</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L3" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="N3" t="s">
         <v>512</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="N3" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B4" t="s">
+        <v>516</v>
+      </c>
+      <c r="C4" t="s">
         <v>517</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>518</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>519</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>520</v>
       </c>
-      <c r="K4" t="s">
-        <v>521</v>
-      </c>
       <c r="L4" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="N4" t="s">
         <v>512</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="N4" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>496</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="C5" t="s">
+        <v>499</v>
+      </c>
+      <c r="D5" t="s">
+        <v>500</v>
+      </c>
+      <c r="E5" t="s">
         <v>497</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="F5" t="s">
+        <v>498</v>
+      </c>
+      <c r="G5" t="s">
         <v>499</v>
       </c>
-      <c r="C5" t="s">
-        <v>500</v>
-      </c>
-      <c r="D5" t="s">
-        <v>501</v>
-      </c>
-      <c r="E5" t="s">
-        <v>498</v>
-      </c>
-      <c r="F5" t="s">
-        <v>499</v>
-      </c>
-      <c r="G5" t="s">
-        <v>500</v>
-      </c>
       <c r="H5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I5" t="s">
         <v>60</v>
@@ -7911,16 +7911,16 @@
         <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L5" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="N5" t="s">
         <v>512</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="N5" t="s">
-        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -7963,160 +7963,160 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C1" t="s">
         <v>523</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>524</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>525</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>526</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>527</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>528</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>529</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>530</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>531</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>532</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>533</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>534</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>535</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>536</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>537</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>538</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>539</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>540</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>541</v>
-      </c>
-      <c r="U1" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B2" t="s">
         <v>543</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>544</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>545</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>546</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>547</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>548</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>549</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>550</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>551</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>552</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>553</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>554</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>555</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>556</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>557</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>558</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>559</v>
       </c>
-      <c r="S2" t="s">
-        <v>560</v>
-      </c>
       <c r="U2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>560</v>
+      </c>
+      <c r="B3" t="s">
         <v>561</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>562</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>315</v>
+      </c>
+      <c r="O3" t="s">
         <v>563</v>
       </c>
-      <c r="D3" t="s">
-        <v>316</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="T3" t="s">
         <v>564</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>565</v>
-      </c>
-      <c r="U3" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>566</v>
+      </c>
+      <c r="O4" t="s">
         <v>567</v>
       </c>
-      <c r="O4" t="s">
+      <c r="T4" t="s">
         <v>568</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>569</v>
-      </c>
-      <c r="U4" t="s">
-        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -8162,70 +8162,70 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C1" t="s">
         <v>523</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>524</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>525</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>526</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>527</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>528</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>529</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>530</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>531</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>532</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>533</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>534</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>535</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>536</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>537</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>538</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>539</v>
       </c>
-      <c r="S1" t="s">
-        <v>540</v>
-      </c>
       <c r="T1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="U1" t="s">
         <v>132</v>
       </c>
       <c r="V1" t="s">
+        <v>570</v>
+      </c>
+      <c r="W1" t="s">
         <v>571</v>
-      </c>
-      <c r="W1" t="s">
-        <v>572</v>
       </c>
       <c r="X1" t="s">
         <v>122</v>
@@ -8233,93 +8233,93 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C2" t="s">
+        <v>548</v>
+      </c>
+      <c r="D2" t="s">
+        <v>572</v>
+      </c>
+      <c r="E2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F2" t="s">
         <v>543</v>
       </c>
-      <c r="B2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C2" t="s">
-        <v>549</v>
-      </c>
-      <c r="D2" t="s">
-        <v>573</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>544</v>
+      </c>
+      <c r="H2" t="s">
         <v>574</v>
       </c>
-      <c r="F2" t="s">
-        <v>544</v>
-      </c>
-      <c r="G2" t="s">
-        <v>545</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>553</v>
+      </c>
+      <c r="J2" t="s">
+        <v>554</v>
+      </c>
+      <c r="K2" t="s">
         <v>575</v>
       </c>
-      <c r="I2" t="s">
-        <v>554</v>
-      </c>
-      <c r="J2" t="s">
-        <v>555</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>550</v>
+      </c>
+      <c r="M2" t="s">
+        <v>551</v>
+      </c>
+      <c r="N2" t="s">
         <v>576</v>
       </c>
-      <c r="L2" t="s">
-        <v>551</v>
-      </c>
-      <c r="M2" t="s">
-        <v>552</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>577</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>578</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>579</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>580</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>542</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="T2" t="s">
-        <v>543</v>
-      </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="X2" t="s">
         <v>582</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="X2" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>585</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>586</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>186</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -8330,45 +8330,45 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="T3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="V3" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="X3" t="s">
         <v>582</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="X3" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>589</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="O4" t="s">
         <v>590</v>
       </c>
-      <c r="O4" t="s">
+      <c r="T4" t="s">
+        <v>569</v>
+      </c>
+      <c r="V4" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="T4" t="s">
-        <v>570</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>592</v>
-      </c>
       <c r="W4" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="X4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -8425,108 +8425,108 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B1" t="s">
         <v>593</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>594</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>595</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>596</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>597</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>598</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>599</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>600</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>601</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>602</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>603</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>604</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>605</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>606</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>607</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>608</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>609</v>
+      </c>
+      <c r="B2" t="s">
         <v>610</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>611</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="6" t="s">
         <v>612</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>613</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" t="s">
         <v>614</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>615</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>616</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>617</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>618</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>619</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>620</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>621</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>622</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>623</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>624</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="10" t="s">
         <v>625</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -8565,121 +8565,121 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B1" t="s">
         <v>593</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>626</v>
+      </c>
+      <c r="D1" t="s">
         <v>594</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>595</v>
+      </c>
+      <c r="F1" t="s">
+        <v>596</v>
+      </c>
+      <c r="G1" t="s">
         <v>627</v>
       </c>
-      <c r="D1" t="s">
-        <v>595</v>
-      </c>
-      <c r="E1" t="s">
-        <v>596</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>597</v>
       </c>
-      <c r="G1" t="s">
-        <v>628</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>598</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>599</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>600</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>601</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>602</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>603</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>604</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>605</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>606</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>607</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>608</v>
-      </c>
-      <c r="S1" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>609</v>
+      </c>
+      <c r="B2" t="s">
         <v>610</v>
       </c>
-      <c r="B2" t="s">
-        <v>611</v>
-      </c>
       <c r="C2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D2" t="str">
         <f>LOWER(C2)</f>
         <v>withdrawn</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H2" t="s">
+        <v>614</v>
+      </c>
+      <c r="I2" t="s">
         <v>615</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>616</v>
       </c>
-      <c r="J2" t="s">
-        <v>617</v>
-      </c>
       <c r="K2" t="s">
+        <v>629</v>
+      </c>
+      <c r="L2" t="s">
         <v>630</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>631</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>632</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>633</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>634</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>635</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>636</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" s="10" t="s">
         <v>637</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -8703,47 +8703,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B1" t="s">
         <v>648</v>
-      </c>
-      <c r="B1" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>82</v>
@@ -8751,170 +8751,170 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
   </sheetData>
@@ -9071,6 +9071,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9079,7 +9090,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9334,18 +9345,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -9353,7 +9364,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9370,15 +9381,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change to Dietitian in social
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA07211-B601-4504-B2CF-B4392460E21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A6D3D5-AFAA-4013-8B30-A863DD23D437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="34" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="34" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -2290,7 +2290,7 @@
     <t>Division of Left Knee Tendon, Open Approach</t>
   </si>
   <si>
-    <t>Diet</t>
+    <t>Dietitian</t>
   </si>
 </sst>
 </file>
@@ -4891,8 +4891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DAC4B0-6F7A-40C4-8629-2F293F19EE6C}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4941,7 +4941,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5237,8 +5237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF82F3D0-82CD-49AF-BA0A-7CEE53FBA6AC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9071,6 +9071,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9325,7 +9334,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
@@ -9336,16 +9345,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9364,7 +9372,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9373,12 +9381,4 @@
     <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change condition to Past medical history
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9098FE-A41D-47A1-9D20-CF2C96472DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184C5E76-630C-4FA7-A836-1A73BA63C57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="46" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="725">
   <si>
     <t>username</t>
   </si>
@@ -1069,9 +1069,6 @@
     <t>cond_notes</t>
   </si>
   <si>
-    <t>Condition</t>
-  </si>
-  <si>
     <t>Erythematous condition</t>
   </si>
   <si>
@@ -2029,9 +2026,6 @@
     <t>08/07/2025</t>
   </si>
   <si>
-    <t>Conditions</t>
-  </si>
-  <si>
     <t>22/07/2025</t>
   </si>
   <si>
@@ -2285,6 +2279,9 @@
   </si>
   <si>
     <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Past Medical History</t>
   </si>
 </sst>
 </file>
@@ -2666,7 +2663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE4FC9F-2982-4FD6-8BD6-4330FF8DA2DE}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2689,31 +2686,31 @@
         <v>279</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2721,7 +2718,7 @@
         <v>279</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -3218,16 +3215,16 @@
         <v>159</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>157</v>
       </c>
       <c r="L2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M2" t="s">
         <v>188</v>
@@ -3539,22 +3536,22 @@
     </row>
     <row r="2" spans="1:48" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>51</v>
@@ -3674,7 +3671,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C2" t="s">
         <v>131</v>
@@ -3737,7 +3734,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C2" t="s">
         <v>116</v>
@@ -3788,7 +3785,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -3858,7 +3855,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>01/12/2025</v>
+        <v>02/12/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -3937,7 +3934,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>01/12/2025</v>
+        <v>02/12/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -4072,13 +4069,13 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>102</v>
@@ -4179,11 +4176,11 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>102</v>
@@ -4249,7 +4246,7 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -4582,7 +4579,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4594,7 +4591,7 @@
         <v>247</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G2" t="s">
         <v>248</v>
@@ -4680,7 +4677,7 @@
         <v>245</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>136</v>
@@ -4739,7 +4736,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B2" t="s">
         <v>255</v>
@@ -4932,7 +4929,7 @@
         <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>261</v>
@@ -4981,7 +4978,7 @@
         <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>263</v>
@@ -5047,7 +5044,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -5137,7 +5134,7 @@
         <v>200</v>
       </c>
       <c r="AH1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -5145,13 +5142,13 @@
         <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E2" t="s">
         <v>71</v>
@@ -5169,10 +5166,10 @@
         <v>102</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>638</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>639</v>
       </c>
       <c r="L2" t="s">
         <v>176</v>
@@ -5205,7 +5202,7 @@
         <v>82</v>
       </c>
       <c r="X2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Y2" t="s">
         <v>104</v>
@@ -5235,7 +5232,7 @@
         <v>201</v>
       </c>
       <c r="AH2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -5274,7 +5271,7 @@
         <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -5320,7 +5317,7 @@
         <v>270</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>268</v>
@@ -5369,7 +5366,7 @@
         <v>270</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>271</v>
@@ -5414,7 +5411,7 @@
         <v>266</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C2" t="s">
         <v>272</v>
@@ -5459,7 +5456,7 @@
         <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>277</v>
@@ -5507,7 +5504,7 @@
         <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>276</v>
@@ -5552,7 +5549,7 @@
         <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" t="s">
         <v>278</v>
@@ -5673,7 +5670,7 @@
         <v>304</v>
       </c>
       <c r="N2" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="O2" t="s">
         <v>302</v>
@@ -5813,7 +5810,7 @@
         <v>304</v>
       </c>
       <c r="N2" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="O2" t="s">
         <v>302</v>
@@ -5847,7 +5844,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5881,22 +5878,22 @@
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>724</v>
+      </c>
+      <c r="B2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>640</v>
       </c>
-      <c r="B2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>642</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F2" t="s">
         <v>324</v>
-      </c>
-      <c r="F2" t="s">
-        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -5945,7 +5942,7 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
@@ -6017,7 +6014,7 @@
         <v>112</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E2" t="s">
         <v>86</v>
@@ -6081,7 +6078,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6115,22 +6112,22 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>724</v>
+      </c>
+      <c r="B2" t="s">
         <v>320</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>323</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -6142,8 +6139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A0A6C0-CF2F-48B8-BAC5-F3E5690001A5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6165,13 +6162,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>724</v>
+      </c>
+      <c r="B2" t="s">
         <v>320</v>
       </c>
-      <c r="B2" t="s">
-        <v>321</v>
-      </c>
       <c r="C2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -6206,21 +6203,21 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>329</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>330</v>
-      </c>
-      <c r="D2" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -6256,21 +6253,21 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>329</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>330</v>
-      </c>
-      <c r="D2" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -6306,13 +6303,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>329</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -6346,67 +6343,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B1" t="s">
+        <v>697</v>
+      </c>
+      <c r="C1" t="s">
         <v>699</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>701</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>703</v>
       </c>
-      <c r="E1" t="s">
-        <v>705</v>
-      </c>
       <c r="F1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G1" t="s">
+        <v>332</v>
+      </c>
+      <c r="H1" t="s">
         <v>333</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>334</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>335</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>336</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>337</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>338</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>339</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>340</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>341</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>342</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>343</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>344</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>345</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>346</v>
-      </c>
-      <c r="U1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -6414,65 +6411,65 @@
         <v>221</v>
       </c>
       <c r="B2" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2" t="s">
         <v>700</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>702</v>
       </c>
-      <c r="D2" t="s">
-        <v>704</v>
-      </c>
       <c r="E2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="G2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H2" s="9" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>01/12/2025</v>
+        <v>02/12/2025</v>
       </c>
       <c r="I2" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" t="s">
         <v>351</v>
       </c>
-      <c r="L2" t="s">
-        <v>352</v>
-      </c>
       <c r="M2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N2" t="s">
         <v>98</v>
       </c>
       <c r="O2" t="s">
+        <v>352</v>
+      </c>
+      <c r="P2" t="s">
         <v>353</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>354</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>355</v>
-      </c>
-      <c r="R2" t="s">
-        <v>356</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>317</v>
       </c>
       <c r="T2" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="U2" t="s">
         <v>357</v>
-      </c>
-      <c r="U2" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -6495,72 +6492,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B1" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D1" t="s">
         <v>299</v>
       </c>
       <c r="E1" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="F1" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="G1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H1" t="s">
         <v>299</v>
       </c>
       <c r="I1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J1" t="s">
         <v>345</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>346</v>
-      </c>
-      <c r="K1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>718</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>719</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>720</v>
-      </c>
       <c r="D2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E2" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="F2" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="G2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>317</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="K2" t="s">
         <v>357</v>
-      </c>
-      <c r="K2" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -6593,58 +6590,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B1" t="s">
+        <v>697</v>
+      </c>
+      <c r="C1" t="s">
         <v>699</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>701</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>703</v>
       </c>
-      <c r="E1" t="s">
-        <v>705</v>
-      </c>
       <c r="F1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H1" t="s">
+        <v>358</v>
+      </c>
+      <c r="I1" t="s">
         <v>359</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K1" t="s">
+        <v>338</v>
+      </c>
+      <c r="L1" t="s">
+        <v>339</v>
+      </c>
+      <c r="M1" t="s">
+        <v>340</v>
+      </c>
+      <c r="N1" t="s">
         <v>360</v>
-      </c>
-      <c r="J1" t="s">
-        <v>338</v>
-      </c>
-      <c r="K1" t="s">
-        <v>339</v>
-      </c>
-      <c r="L1" t="s">
-        <v>340</v>
-      </c>
-      <c r="M1" t="s">
-        <v>341</v>
-      </c>
-      <c r="N1" t="s">
-        <v>361</v>
       </c>
       <c r="O1" t="s">
         <v>299</v>
       </c>
       <c r="P1" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q1" t="s">
         <v>345</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>346</v>
-      </c>
-      <c r="R1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -6652,56 +6649,56 @@
         <v>221</v>
       </c>
       <c r="B2" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2" t="s">
         <v>700</v>
       </c>
-      <c r="C2" t="s">
-        <v>702</v>
-      </c>
       <c r="D2" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E2" t="s">
+        <v>706</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>708</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>710</v>
-      </c>
       <c r="G2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H2" s="9" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>01/12/2025</v>
+        <v>02/12/2025</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="J2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L2" t="s">
         <v>98</v>
       </c>
       <c r="M2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>317</v>
       </c>
       <c r="Q2" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="R2" t="s">
         <v>357</v>
-      </c>
-      <c r="R2" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -6742,93 +6739,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D1" t="s">
         <v>370</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>371</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>372</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>373</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>374</v>
       </c>
-      <c r="H1" t="s">
-        <v>375</v>
-      </c>
       <c r="I1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="N1" t="s">
+        <v>391</v>
+      </c>
+      <c r="O1" t="s">
         <v>392</v>
-      </c>
-      <c r="O1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F2" t="s">
+        <v>378</v>
+      </c>
+      <c r="G2" t="s">
+        <v>379</v>
+      </c>
+      <c r="H2" t="s">
+        <v>380</v>
+      </c>
+      <c r="I2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J2" t="s">
+        <v>384</v>
+      </c>
+      <c r="K2" t="s">
+        <v>386</v>
+      </c>
+      <c r="L2" t="s">
+        <v>388</v>
+      </c>
+      <c r="M2" t="s">
+        <v>390</v>
+      </c>
+      <c r="N2" t="s">
         <v>395</v>
       </c>
-      <c r="B2" t="s">
-        <v>369</v>
-      </c>
-      <c r="C2" t="s">
-        <v>376</v>
-      </c>
-      <c r="D2" t="s">
-        <v>377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>378</v>
-      </c>
-      <c r="F2" t="s">
-        <v>379</v>
-      </c>
-      <c r="G2" t="s">
-        <v>380</v>
-      </c>
-      <c r="H2" t="s">
-        <v>381</v>
-      </c>
-      <c r="I2" t="s">
-        <v>383</v>
-      </c>
-      <c r="J2" t="s">
-        <v>385</v>
-      </c>
-      <c r="K2" t="s">
-        <v>387</v>
-      </c>
-      <c r="L2" t="s">
-        <v>389</v>
-      </c>
-      <c r="M2" t="s">
-        <v>391</v>
-      </c>
-      <c r="N2" t="s">
-        <v>396</v>
-      </c>
       <c r="O2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="P2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -6869,93 +6866,93 @@
         <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D1" t="s">
         <v>370</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>371</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>372</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>373</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>374</v>
       </c>
-      <c r="H1" t="s">
-        <v>375</v>
-      </c>
       <c r="I1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="N1" t="s">
+        <v>391</v>
+      </c>
+      <c r="O1" t="s">
         <v>392</v>
-      </c>
-      <c r="O1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D2" t="s">
         <v>376</v>
       </c>
-      <c r="D2" t="s">
-        <v>377</v>
-      </c>
       <c r="E2" t="s">
+        <v>396</v>
+      </c>
+      <c r="F2" t="s">
+        <v>378</v>
+      </c>
+      <c r="G2" t="s">
+        <v>379</v>
+      </c>
+      <c r="H2" t="s">
         <v>397</v>
       </c>
-      <c r="F2" t="s">
-        <v>379</v>
-      </c>
-      <c r="G2" t="s">
-        <v>380</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J2" t="s">
+        <v>384</v>
+      </c>
+      <c r="K2" t="s">
         <v>398</v>
       </c>
-      <c r="I2" t="s">
-        <v>383</v>
-      </c>
-      <c r="J2" t="s">
-        <v>385</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>388</v>
+      </c>
+      <c r="M2" t="s">
+        <v>390</v>
+      </c>
+      <c r="N2" t="s">
         <v>399</v>
       </c>
-      <c r="L2" t="s">
-        <v>389</v>
-      </c>
-      <c r="M2" t="s">
-        <v>391</v>
-      </c>
-      <c r="N2" t="s">
-        <v>400</v>
-      </c>
       <c r="O2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="P2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -7043,55 +7040,55 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B1" t="s">
         <v>401</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>402</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>403</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>404</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>405</v>
       </c>
-      <c r="F1" t="s">
-        <v>406</v>
-      </c>
       <c r="G1" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" t="s">
         <v>409</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>410</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>411</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>412</v>
       </c>
-      <c r="K1" t="s">
-        <v>413</v>
-      </c>
       <c r="L1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>01/12/2025</v>
+        <v>02/12/2025</v>
       </c>
       <c r="C2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" t="s">
         <v>407</v>
-      </c>
-      <c r="D2" t="s">
-        <v>408</v>
       </c>
       <c r="E2" t="s">
         <v>303</v>
@@ -7100,19 +7097,19 @@
         <v>116</v>
       </c>
       <c r="H2" t="s">
+        <v>413</v>
+      </c>
+      <c r="I2" t="s">
         <v>414</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>415</v>
       </c>
-      <c r="J2" t="s">
-        <v>416</v>
-      </c>
       <c r="K2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -7280,16 +7277,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>430</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -7326,66 +7323,66 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B1" t="s">
         <v>432</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>433</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>434</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>435</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>436</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>437</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>438</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>439</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>440</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>441</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>442</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>443</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>444</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>445</v>
-      </c>
-      <c r="O1" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B2" t="s">
         <v>447</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>448</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>449</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="6" t="s">
         <v>450</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>451</v>
       </c>
       <c r="F2" t="str">
         <f>LOWER(G2)</f>
@@ -7399,7 +7396,7 @@
         <v>internal</v>
       </c>
       <c r="I2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J2" t="str">
         <f>LOWER(K2)</f>
@@ -7409,17 +7406,17 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="M2" t="str">
         <f>LOWER(N2)</f>
         <v>implanted</v>
       </c>
       <c r="N2" t="s">
+        <v>453</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>454</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -7457,86 +7454,86 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B1" t="s">
         <v>432</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>433</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>434</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>455</v>
+      </c>
+      <c r="F1" t="s">
         <v>435</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>436</v>
+      </c>
+      <c r="H1" t="s">
+        <v>437</v>
+      </c>
+      <c r="I1" t="s">
+        <v>438</v>
+      </c>
+      <c r="J1" t="s">
+        <v>439</v>
+      </c>
+      <c r="K1" t="s">
+        <v>440</v>
+      </c>
+      <c r="L1" t="s">
+        <v>441</v>
+      </c>
+      <c r="M1" t="s">
+        <v>442</v>
+      </c>
+      <c r="N1" t="s">
+        <v>443</v>
+      </c>
+      <c r="O1" t="s">
+        <v>444</v>
+      </c>
+      <c r="P1" t="s">
         <v>456</v>
-      </c>
-      <c r="F1" t="s">
-        <v>436</v>
-      </c>
-      <c r="G1" t="s">
-        <v>437</v>
-      </c>
-      <c r="H1" t="s">
-        <v>438</v>
-      </c>
-      <c r="I1" t="s">
-        <v>439</v>
-      </c>
-      <c r="J1" t="s">
-        <v>440</v>
-      </c>
-      <c r="K1" t="s">
-        <v>441</v>
-      </c>
-      <c r="L1" t="s">
-        <v>442</v>
-      </c>
-      <c r="M1" t="s">
-        <v>443</v>
-      </c>
-      <c r="N1" t="s">
-        <v>444</v>
-      </c>
-      <c r="O1" t="s">
-        <v>445</v>
-      </c>
-      <c r="P1" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2" t="s">
         <v>458</v>
       </c>
-      <c r="C2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>459</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="6" t="s">
         <v>460</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>461</v>
       </c>
       <c r="G2" t="str">
         <f>SUBSTITUTE(LOWER(H2)," ","")</f>
         <v>firststage</v>
       </c>
       <c r="H2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I2" t="str">
         <f>LOWER(J2)</f>
         <v>external</v>
       </c>
       <c r="J2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K2" t="str">
         <f>LOWER(L2)</f>
@@ -7546,7 +7543,7 @@
         <v>184</v>
       </c>
       <c r="M2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N2" t="str">
         <f>LOWER(O2)</f>
@@ -7556,7 +7553,7 @@
         <v>205</v>
       </c>
       <c r="P2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -7589,126 +7586,126 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" t="s">
         <v>466</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>467</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>468</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>469</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>470</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>471</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>472</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>473</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>474</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>475</v>
-      </c>
-      <c r="K1" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B2" t="s">
         <v>477</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>478</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>479</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>480</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>481</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>482</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>483</v>
-      </c>
-      <c r="K2" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B3" t="s">
         <v>485</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>486</v>
-      </c>
-      <c r="C3" t="s">
-        <v>487</v>
       </c>
       <c r="D3" t="s">
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>488</v>
+      </c>
+      <c r="B4" t="s">
         <v>489</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>490</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>491</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>492</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>493</v>
-      </c>
-      <c r="K4" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>494</v>
+      </c>
+      <c r="B5" t="s">
         <v>495</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" t="s">
         <v>497</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>498</v>
       </c>
-      <c r="E5" t="s">
-        <v>499</v>
-      </c>
       <c r="F5" t="s">
+        <v>495</v>
+      </c>
+      <c r="G5" t="s">
         <v>496</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>497</v>
-      </c>
-      <c r="H5" t="s">
-        <v>498</v>
       </c>
       <c r="I5" t="s">
         <v>100</v>
@@ -7717,7 +7714,7 @@
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7757,43 +7754,43 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" t="s">
         <v>466</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>467</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>468</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>469</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>470</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>471</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>472</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>473</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>474</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>475</v>
       </c>
-      <c r="K1" t="s">
-        <v>476</v>
-      </c>
       <c r="L1" t="s">
+        <v>500</v>
+      </c>
+      <c r="M1" t="s">
         <v>501</v>
-      </c>
-      <c r="M1" t="s">
-        <v>502</v>
       </c>
       <c r="N1" t="s">
         <v>122</v>
@@ -7801,118 +7798,118 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B2" t="s">
+        <v>502</v>
+      </c>
+      <c r="C2" t="s">
         <v>503</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>504</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>505</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>506</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>507</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>508</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="N2" t="s">
         <v>510</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="N2" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C3" t="s">
         <v>512</v>
-      </c>
-      <c r="C3" t="s">
-        <v>513</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L3" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="N3" t="s">
         <v>510</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="N3" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B4" t="s">
+        <v>514</v>
+      </c>
+      <c r="C4" t="s">
         <v>515</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>516</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>517</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>518</v>
       </c>
-      <c r="K4" t="s">
-        <v>519</v>
-      </c>
       <c r="L4" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="N4" t="s">
         <v>510</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="N4" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>494</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="C5" t="s">
+        <v>497</v>
+      </c>
+      <c r="D5" t="s">
+        <v>498</v>
+      </c>
+      <c r="E5" t="s">
         <v>495</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="F5" t="s">
+        <v>496</v>
+      </c>
+      <c r="G5" t="s">
         <v>497</v>
       </c>
-      <c r="C5" t="s">
-        <v>498</v>
-      </c>
-      <c r="D5" t="s">
-        <v>499</v>
-      </c>
-      <c r="E5" t="s">
-        <v>496</v>
-      </c>
-      <c r="F5" t="s">
-        <v>497</v>
-      </c>
-      <c r="G5" t="s">
-        <v>498</v>
-      </c>
       <c r="H5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I5" t="s">
         <v>60</v>
@@ -7921,16 +7918,16 @@
         <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L5" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="N5" t="s">
         <v>510</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="N5" t="s">
-        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -7973,160 +7970,160 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C1" t="s">
         <v>521</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>522</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>523</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>524</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>525</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>526</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>527</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>528</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>529</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>530</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>531</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>532</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>533</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>534</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>535</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>536</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>537</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>538</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>539</v>
-      </c>
-      <c r="U1" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B2" t="s">
         <v>541</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>542</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>543</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>544</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>545</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>546</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>547</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>548</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>549</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>550</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>551</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>552</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>553</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>554</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>555</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>556</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>557</v>
       </c>
-      <c r="S2" t="s">
-        <v>558</v>
-      </c>
       <c r="U2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>558</v>
+      </c>
+      <c r="B3" t="s">
         <v>559</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>560</v>
-      </c>
-      <c r="C3" t="s">
-        <v>561</v>
       </c>
       <c r="D3" t="s">
         <v>315</v>
       </c>
       <c r="O3" t="s">
+        <v>561</v>
+      </c>
+      <c r="T3" t="s">
         <v>562</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>563</v>
-      </c>
-      <c r="U3" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>564</v>
+      </c>
+      <c r="O4" t="s">
         <v>565</v>
       </c>
-      <c r="O4" t="s">
+      <c r="T4" t="s">
         <v>566</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>567</v>
-      </c>
-      <c r="U4" t="s">
-        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -8172,70 +8169,70 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C1" t="s">
         <v>521</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>522</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>523</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>524</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>525</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>526</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>527</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>528</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>529</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>530</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>531</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>532</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>533</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>534</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>535</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>536</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>537</v>
       </c>
-      <c r="S1" t="s">
-        <v>538</v>
-      </c>
       <c r="T1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="U1" t="s">
         <v>132</v>
       </c>
       <c r="V1" t="s">
+        <v>568</v>
+      </c>
+      <c r="W1" t="s">
         <v>569</v>
-      </c>
-      <c r="W1" t="s">
-        <v>570</v>
       </c>
       <c r="X1" t="s">
         <v>122</v>
@@ -8243,93 +8240,93 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C2" t="s">
+        <v>546</v>
+      </c>
+      <c r="D2" t="s">
+        <v>570</v>
+      </c>
+      <c r="E2" t="s">
+        <v>571</v>
+      </c>
+      <c r="F2" t="s">
         <v>541</v>
       </c>
-      <c r="B2" t="s">
-        <v>546</v>
-      </c>
-      <c r="C2" t="s">
-        <v>547</v>
-      </c>
-      <c r="D2" t="s">
-        <v>571</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>542</v>
+      </c>
+      <c r="H2" t="s">
         <v>572</v>
       </c>
-      <c r="F2" t="s">
-        <v>542</v>
-      </c>
-      <c r="G2" t="s">
-        <v>543</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>551</v>
+      </c>
+      <c r="J2" t="s">
+        <v>552</v>
+      </c>
+      <c r="K2" t="s">
         <v>573</v>
       </c>
-      <c r="I2" t="s">
-        <v>552</v>
-      </c>
-      <c r="J2" t="s">
-        <v>553</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>548</v>
+      </c>
+      <c r="M2" t="s">
+        <v>549</v>
+      </c>
+      <c r="N2" t="s">
         <v>574</v>
       </c>
-      <c r="L2" t="s">
-        <v>549</v>
-      </c>
-      <c r="M2" t="s">
-        <v>550</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>575</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>576</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>577</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>578</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>540</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="T2" t="s">
-        <v>541</v>
-      </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="X2" t="s">
         <v>580</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>580</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>580</v>
-      </c>
-      <c r="X2" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>583</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>584</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>186</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -8340,45 +8337,45 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="T3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="V3" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="X3" t="s">
         <v>580</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>580</v>
-      </c>
-      <c r="X3" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>587</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="O4" t="s">
         <v>588</v>
       </c>
-      <c r="O4" t="s">
+      <c r="T4" t="s">
+        <v>567</v>
+      </c>
+      <c r="V4" s="5" t="s">
         <v>589</v>
       </c>
-      <c r="T4" t="s">
-        <v>568</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>590</v>
-      </c>
       <c r="W4" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="X4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -8435,108 +8432,108 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B1" t="s">
         <v>591</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>592</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>593</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>594</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>595</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>596</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>597</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>598</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>599</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>600</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>601</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>602</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>603</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>604</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>605</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>606</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B2" t="s">
         <v>608</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>609</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="6" t="s">
         <v>610</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>611</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" t="s">
         <v>612</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>613</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>614</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>615</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>616</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>617</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>618</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>619</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>620</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>621</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>622</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="10" t="s">
         <v>623</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>624</v>
       </c>
     </row>
   </sheetData>
@@ -8575,121 +8572,121 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B1" t="s">
         <v>591</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>624</v>
+      </c>
+      <c r="D1" t="s">
         <v>592</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>593</v>
+      </c>
+      <c r="F1" t="s">
+        <v>594</v>
+      </c>
+      <c r="G1" t="s">
         <v>625</v>
       </c>
-      <c r="D1" t="s">
-        <v>593</v>
-      </c>
-      <c r="E1" t="s">
-        <v>594</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>595</v>
       </c>
-      <c r="G1" t="s">
-        <v>626</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>596</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>597</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>598</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>599</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>600</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>601</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>602</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>603</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>604</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>605</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>606</v>
-      </c>
-      <c r="S1" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B2" t="s">
         <v>608</v>
       </c>
-      <c r="B2" t="s">
-        <v>609</v>
-      </c>
       <c r="C2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D2" t="str">
         <f>LOWER(C2)</f>
         <v>withdrawn</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H2" t="s">
+        <v>612</v>
+      </c>
+      <c r="I2" t="s">
         <v>613</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>614</v>
       </c>
-      <c r="J2" t="s">
-        <v>615</v>
-      </c>
       <c r="K2" t="s">
+        <v>627</v>
+      </c>
+      <c r="L2" t="s">
         <v>628</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>629</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>630</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>631</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>632</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>633</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>634</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" s="10" t="s">
         <v>635</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -8713,47 +8710,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>82</v>
@@ -8761,135 +8758,135 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>315</v>
@@ -8897,26 +8894,26 @@
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -9073,26 +9070,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9347,26 +9324,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9383,4 +9361,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add diet for social
</commit_message>
<xml_diff>
--- a/ExcelFiles/PatientSummary.xlsx
+++ b/ExcelFiles/PatientSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184C5E76-630C-4FA7-A836-1A73BA63C57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF8A7E9-829D-48BF-8B60-556208D337FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="46" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="34" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="2" r:id="rId1"/>
@@ -2272,9 +2272,6 @@
     <t>Division of Left Knee Tendon, Open Approach</t>
   </si>
   <si>
-    <t>Dietitian</t>
-  </si>
-  <si>
     <t>Height (cm) (cm)</t>
   </si>
   <si>
@@ -2282,6 +2279,9 @@
   </si>
   <si>
     <t>Past Medical History</t>
+  </si>
+  <si>
+    <t>Diet</t>
   </si>
 </sst>
 </file>
@@ -3855,7 +3855,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>02/12/2025</v>
+        <v>05/12/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>197</v>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>02/12/2025</v>
+        <v>05/12/2025</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>198</v>
@@ -4180,7 +4180,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45993</v>
+        <v>45996</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>102</v>
@@ -4929,7 +4929,7 @@
         <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>261</v>
@@ -4978,7 +4978,7 @@
         <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>263</v>
@@ -5244,7 +5244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF82F3D0-82CD-49AF-BA0A-7CEE53FBA6AC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5271,7 +5271,7 @@
         <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
@@ -5878,7 +5878,7 @@
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B2" t="s">
         <v>320</v>
@@ -6112,7 +6112,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B2" t="s">
         <v>320</v>
@@ -6139,7 +6139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A0A6C0-CF2F-48B8-BAC5-F3E5690001A5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6162,7 +6162,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B2" t="s">
         <v>320</v>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="H2" s="9" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>02/12/2025</v>
+        <v>05/12/2025</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>348</v>
@@ -6668,7 +6668,7 @@
       </c>
       <c r="H2" s="9" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>02/12/2025</v>
+        <v>05/12/2025</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>709</v>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="B2" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "DD/MM/YYYY")</f>
-        <v>02/12/2025</v>
+        <v>05/12/2025</v>
       </c>
       <c r="C2" t="s">
         <v>406</v>
@@ -8782,7 +8782,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>674</v>
@@ -8910,7 +8910,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>687</v>
@@ -9070,6 +9070,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -9324,7 +9333,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
@@ -9335,16 +9344,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1EC2FBF-A56D-40AC-8C09-CB1DCD191DD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9363,7 +9371,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE0B556D-2173-4F7C-9F53-AE9A9D15CB9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9372,12 +9380,4 @@
     <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101DBEFA-2EFF-47B2-92EB-3E72B43EE2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>